<commit_message>
Update PDS Category Assignment files Some color token assignments have been updated
</commit_message>
<xml_diff>
--- a/Cartography/POI/PDS_Category_Assignment.xlsx
+++ b/Cartography/POI/PDS_Category_Assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauragar/OneDrive - HERE Global B.V/HDS/Iconography/PDS Alignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmcs-my.sharepoint.com/personal/alvaro_lauragarcia_here_com/Documents/HDS/Iconography/PDS Alignment/Color tokens adjustments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C2CA8-F74D-C740-9999-B40E43AF3730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{CB3C2CA8-F74D-C740-9999-B40E43AF3730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{02DDAF2A-AC11-0F45-913C-496CA934E2CA}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C64EB798-04F6-AE43-9DCC-0EA02E11247A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{C64EB798-04F6-AE43-9DCC-0EA02E11247A}"/>
   </bookViews>
   <sheets>
     <sheet name="PDS_Category_Assignment" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="1021">
   <si>
     <t>PDS Category name</t>
   </si>
@@ -3729,6 +3729,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3738,6 +3747,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3745,21 +3760,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -25335,8 +25335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693BBA9B-95F3-BD4A-928B-DD81DFE8C409}">
   <dimension ref="A1:H424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G415" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B406" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D413" sqref="D413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="50" customHeight="1" outlineLevelCol="1"/>
@@ -25399,10 +25399,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="50" customHeight="1">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="61" t="s">
         <v>825</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="61" t="s">
         <v>830</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -25423,8 +25423,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="50" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
@@ -25443,8 +25443,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="50" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
@@ -25463,8 +25463,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="50" customHeight="1">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
@@ -25483,8 +25483,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="50" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
@@ -25503,8 +25503,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="50" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
@@ -25523,8 +25523,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="50" customHeight="1">
-      <c r="A9" s="64"/>
-      <c r="B9" s="64"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
@@ -25543,8 +25543,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="50" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
@@ -25563,8 +25563,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="50" customHeight="1">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
@@ -25583,8 +25583,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="50" customHeight="1">
-      <c r="A12" s="64"/>
-      <c r="B12" s="64" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="61" t="s">
         <v>831</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -25605,8 +25605,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="50" customHeight="1">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="8" t="s">
         <v>23</v>
       </c>
@@ -25625,8 +25625,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="50" customHeight="1">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
@@ -25645,8 +25645,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="50" customHeight="1">
-      <c r="A15" s="64"/>
-      <c r="B15" s="64"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
@@ -25665,10 +25665,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="50" customHeight="1">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="60" t="s">
         <v>828</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="60" t="s">
         <v>833</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -25689,8 +25689,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="50" customHeight="1">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
@@ -25709,8 +25709,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="50" customHeight="1">
-      <c r="A18" s="63"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="8" t="s">
         <v>33</v>
       </c>
@@ -25729,8 +25729,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="50" customHeight="1">
-      <c r="A19" s="63"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="8" t="s">
         <v>35</v>
       </c>
@@ -25749,8 +25749,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="50" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="8" t="s">
         <v>37</v>
       </c>
@@ -25769,8 +25769,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="50" customHeight="1">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
@@ -25789,8 +25789,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="50" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="8" t="s">
         <v>41</v>
       </c>
@@ -25809,8 +25809,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="50" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="8" t="s">
         <v>43</v>
       </c>
@@ -25829,8 +25829,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="50" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="B24" s="63"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="8" t="s">
         <v>45</v>
       </c>
@@ -25849,8 +25849,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="50" customHeight="1">
-      <c r="A25" s="63"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="13" t="s">
         <v>47</v>
       </c>
@@ -25868,8 +25868,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="50" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="60"/>
       <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
@@ -25888,8 +25888,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="50" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="63"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="8" t="s">
         <v>51</v>
       </c>
@@ -25908,7 +25908,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="50" customHeight="1">
-      <c r="A28" s="63"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="14" t="s">
         <v>834</v>
       </c>
@@ -25930,8 +25930,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="50" customHeight="1">
-      <c r="A29" s="63"/>
-      <c r="B29" s="63" t="s">
+      <c r="A29" s="60"/>
+      <c r="B29" s="60" t="s">
         <v>835</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -25952,8 +25952,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="50" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="B30" s="63"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="8" t="s">
         <v>57</v>
       </c>
@@ -25972,8 +25972,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="50" customHeight="1">
-      <c r="A31" s="63"/>
-      <c r="B31" s="63" t="s">
+      <c r="A31" s="60"/>
+      <c r="B31" s="60" t="s">
         <v>836</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -25994,8 +25994,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="50" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="B32" s="63"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="8" t="s">
         <v>61</v>
       </c>
@@ -26014,8 +26014,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="50" customHeight="1">
-      <c r="A33" s="63"/>
-      <c r="B33" s="63"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="8" t="s">
         <v>63</v>
       </c>
@@ -26034,10 +26034,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="50" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="57" t="s">
         <v>832</v>
       </c>
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="60" t="s">
         <v>839</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -26058,8 +26058,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="50" customHeight="1">
-      <c r="A35" s="55"/>
-      <c r="B35" s="63"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="8" t="s">
         <v>67</v>
       </c>
@@ -26078,8 +26078,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="50" customHeight="1">
-      <c r="A36" s="55"/>
-      <c r="B36" s="63"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="8" t="s">
         <v>69</v>
       </c>
@@ -26098,8 +26098,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="50" customHeight="1">
-      <c r="A37" s="55"/>
-      <c r="B37" s="63"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="8" t="s">
         <v>71</v>
       </c>
@@ -26118,8 +26118,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="50" customHeight="1">
-      <c r="A38" s="55"/>
-      <c r="B38" s="63"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="60"/>
       <c r="C38" s="8" t="s">
         <v>1012</v>
       </c>
@@ -26130,12 +26130,16 @@
         <v>930</v>
       </c>
       <c r="F38" s="10"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="40"/>
+      <c r="G38" s="18" t="s">
+        <v>990</v>
+      </c>
+      <c r="H38" s="40" t="s">
+        <v>991</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="50" customHeight="1">
-      <c r="A39" s="55"/>
-      <c r="B39" s="63"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="60"/>
       <c r="C39" s="8" t="s">
         <v>73</v>
       </c>
@@ -26154,8 +26158,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="50" customHeight="1">
-      <c r="A40" s="55"/>
-      <c r="B40" s="63"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="8" t="s">
         <v>75</v>
       </c>
@@ -26174,8 +26178,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="50" customHeight="1">
-      <c r="A41" s="55"/>
-      <c r="B41" s="63"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="8" t="s">
         <v>77</v>
       </c>
@@ -26194,8 +26198,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="50" customHeight="1">
-      <c r="A42" s="55"/>
-      <c r="B42" s="63"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="60"/>
       <c r="C42" s="8" t="s">
         <v>79</v>
       </c>
@@ -26214,8 +26218,8 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="50" customHeight="1">
-      <c r="A43" s="55"/>
-      <c r="B43" s="63" t="s">
+      <c r="A43" s="58"/>
+      <c r="B43" s="60" t="s">
         <v>840</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -26236,8 +26240,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="50" customHeight="1">
-      <c r="A44" s="55"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="8" t="s">
         <v>83</v>
       </c>
@@ -26256,8 +26260,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="50" customHeight="1">
-      <c r="A45" s="55"/>
-      <c r="B45" s="63"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="60"/>
       <c r="C45" s="8" t="s">
         <v>85</v>
       </c>
@@ -26276,8 +26280,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="50" customHeight="1">
-      <c r="A46" s="55"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="8" t="s">
         <v>87</v>
       </c>
@@ -26296,8 +26300,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="50" customHeight="1">
-      <c r="A47" s="55"/>
-      <c r="B47" s="63"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="60"/>
       <c r="C47" s="8" t="s">
         <v>89</v>
       </c>
@@ -26316,8 +26320,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="50" customHeight="1">
-      <c r="A48" s="55"/>
-      <c r="B48" s="60" t="s">
+      <c r="A48" s="58"/>
+      <c r="B48" s="54" t="s">
         <v>841</v>
       </c>
       <c r="C48" s="8" t="s">
@@ -26330,16 +26334,16 @@
         <v>960</v>
       </c>
       <c r="F48" s="10"/>
-      <c r="G48" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H48" s="40" t="s">
-        <v>991</v>
+      <c r="G48" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H48" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="50" customHeight="1">
-      <c r="A49" s="55"/>
-      <c r="B49" s="61"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="8" t="s">
         <v>93</v>
       </c>
@@ -26350,16 +26354,16 @@
         <v>960</v>
       </c>
       <c r="F49" s="10"/>
-      <c r="G49" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H49" s="40" t="s">
-        <v>991</v>
+      <c r="G49" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H49" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="50" customHeight="1">
-      <c r="A50" s="55"/>
-      <c r="B50" s="61"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="8" t="s">
         <v>95</v>
       </c>
@@ -26370,16 +26374,16 @@
         <v>960</v>
       </c>
       <c r="F50" s="10"/>
-      <c r="G50" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H50" s="40" t="s">
-        <v>991</v>
+      <c r="G50" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H50" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="50" customHeight="1">
-      <c r="A51" s="55"/>
-      <c r="B51" s="61"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="8" t="s">
         <v>97</v>
       </c>
@@ -26390,16 +26394,16 @@
         <v>960</v>
       </c>
       <c r="F51" s="10"/>
-      <c r="G51" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H51" s="40" t="s">
-        <v>991</v>
+      <c r="G51" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H51" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="50" customHeight="1">
-      <c r="A52" s="55"/>
-      <c r="B52" s="61"/>
+      <c r="A52" s="58"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="8" t="s">
         <v>99</v>
       </c>
@@ -26410,16 +26414,16 @@
         <v>960</v>
       </c>
       <c r="F52" s="10"/>
-      <c r="G52" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H52" s="40" t="s">
-        <v>991</v>
+      <c r="G52" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H52" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="50" customHeight="1">
-      <c r="A53" s="55"/>
-      <c r="B53" s="61"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="55"/>
       <c r="C53" s="8" t="s">
         <v>101</v>
       </c>
@@ -26430,16 +26434,16 @@
         <v>960</v>
       </c>
       <c r="F53" s="10"/>
-      <c r="G53" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H53" s="40" t="s">
-        <v>991</v>
+      <c r="G53" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H53" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="50" customHeight="1">
-      <c r="A54" s="55"/>
-      <c r="B54" s="61"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26450,16 +26454,16 @@
         <v>960</v>
       </c>
       <c r="F54" s="34"/>
-      <c r="G54" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H54" s="40" t="s">
-        <v>991</v>
+      <c r="G54" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H54" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="50" customHeight="1">
-      <c r="A55" s="55"/>
-      <c r="B55" s="61"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="8" t="s">
         <v>103</v>
       </c>
@@ -26470,16 +26474,16 @@
         <v>960</v>
       </c>
       <c r="F55" s="10"/>
-      <c r="G55" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H55" s="40" t="s">
-        <v>991</v>
+      <c r="G55" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H55" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="50" customHeight="1">
-      <c r="A56" s="55"/>
-      <c r="B56" s="61"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="8" t="s">
         <v>105</v>
       </c>
@@ -26490,16 +26494,16 @@
         <v>960</v>
       </c>
       <c r="F56" s="10"/>
-      <c r="G56" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H56" s="40" t="s">
-        <v>991</v>
+      <c r="G56" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H56" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="50" customHeight="1">
-      <c r="A57" s="56"/>
-      <c r="B57" s="62"/>
+      <c r="A57" s="59"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="35" t="s">
         <v>906</v>
       </c>
@@ -26510,18 +26514,18 @@
         <v>960</v>
       </c>
       <c r="F57" s="10"/>
-      <c r="G57" s="18" t="s">
-        <v>990</v>
-      </c>
-      <c r="H57" s="40" t="s">
-        <v>991</v>
+      <c r="G57" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H57" s="51" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="50" customHeight="1">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="57" t="s">
         <v>842</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="57" t="s">
         <v>843</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -26542,8 +26546,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="50" customHeight="1">
-      <c r="A59" s="55"/>
-      <c r="B59" s="55"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="8" t="s">
         <v>109</v>
       </c>
@@ -26562,8 +26566,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="50" customHeight="1">
-      <c r="A60" s="55"/>
-      <c r="B60" s="55"/>
+      <c r="A60" s="58"/>
+      <c r="B60" s="58"/>
       <c r="C60" s="8" t="s">
         <v>111</v>
       </c>
@@ -26582,8 +26586,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="50" customHeight="1">
-      <c r="A61" s="55"/>
-      <c r="B61" s="55"/>
+      <c r="A61" s="58"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="8" t="s">
         <v>113</v>
       </c>
@@ -26602,8 +26606,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="50" customHeight="1">
-      <c r="A62" s="55"/>
-      <c r="B62" s="55"/>
+      <c r="A62" s="58"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="8" t="s">
         <v>115</v>
       </c>
@@ -26622,8 +26626,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="50" customHeight="1">
-      <c r="A63" s="55"/>
-      <c r="B63" s="55"/>
+      <c r="A63" s="58"/>
+      <c r="B63" s="58"/>
       <c r="C63" s="8" t="s">
         <v>117</v>
       </c>
@@ -26642,8 +26646,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="50" customHeight="1">
-      <c r="A64" s="55"/>
-      <c r="B64" s="56"/>
+      <c r="A64" s="58"/>
+      <c r="B64" s="59"/>
       <c r="C64" s="8" t="s">
         <v>119</v>
       </c>
@@ -26662,8 +26666,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="50" customHeight="1">
-      <c r="A65" s="55"/>
-      <c r="B65" s="54" t="s">
+      <c r="A65" s="58"/>
+      <c r="B65" s="57" t="s">
         <v>844</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -26684,8 +26688,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="50" customHeight="1">
-      <c r="A66" s="55"/>
-      <c r="B66" s="55"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="58"/>
       <c r="C66" s="8" t="s">
         <v>123</v>
       </c>
@@ -26704,8 +26708,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="50" customHeight="1">
-      <c r="A67" s="55"/>
-      <c r="B67" s="56"/>
+      <c r="A67" s="58"/>
+      <c r="B67" s="59"/>
       <c r="C67" s="8" t="s">
         <v>125</v>
       </c>
@@ -26724,7 +26728,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="50" customHeight="1">
-      <c r="A68" s="55"/>
+      <c r="A68" s="58"/>
       <c r="B68" s="14" t="s">
         <v>845</v>
       </c>
@@ -26746,7 +26750,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="50" customHeight="1">
-      <c r="A69" s="55"/>
+      <c r="A69" s="58"/>
       <c r="B69" s="14" t="s">
         <v>846</v>
       </c>
@@ -26760,15 +26764,15 @@
         <v>932</v>
       </c>
       <c r="F69" s="10"/>
-      <c r="G69" s="19" t="s">
-        <v>992</v>
-      </c>
-      <c r="H69" s="41" t="s">
-        <v>993</v>
+      <c r="G69" s="23" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H69" s="47" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="50" customHeight="1">
-      <c r="A70" s="56"/>
+      <c r="A70" s="59"/>
       <c r="B70" s="14" t="s">
         <v>847</v>
       </c>
@@ -26782,18 +26786,18 @@
         <v>932</v>
       </c>
       <c r="F70" s="10"/>
-      <c r="G70" s="19" t="s">
-        <v>992</v>
-      </c>
-      <c r="H70" s="41" t="s">
-        <v>993</v>
+      <c r="G70" s="23" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H70" s="47" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="50" customHeight="1">
-      <c r="A71" s="54" t="s">
+      <c r="A71" s="57" t="s">
         <v>848</v>
       </c>
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="57" t="s">
         <v>850</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -26814,8 +26818,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="50" customHeight="1">
-      <c r="A72" s="55"/>
-      <c r="B72" s="55"/>
+      <c r="A72" s="58"/>
+      <c r="B72" s="58"/>
       <c r="C72" s="8" t="s">
         <v>135</v>
       </c>
@@ -26834,8 +26838,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="50" customHeight="1">
-      <c r="A73" s="55"/>
-      <c r="B73" s="56"/>
+      <c r="A73" s="58"/>
+      <c r="B73" s="59"/>
       <c r="C73" s="8" t="s">
         <v>137</v>
       </c>
@@ -26854,8 +26858,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="50" customHeight="1">
-      <c r="A74" s="55"/>
-      <c r="B74" s="54" t="s">
+      <c r="A74" s="58"/>
+      <c r="B74" s="57" t="s">
         <v>849</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -26876,8 +26880,8 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="50" customHeight="1">
-      <c r="A75" s="55"/>
-      <c r="B75" s="55"/>
+      <c r="A75" s="58"/>
+      <c r="B75" s="58"/>
       <c r="C75" s="8" t="s">
         <v>141</v>
       </c>
@@ -26896,8 +26900,8 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="50" customHeight="1">
-      <c r="A76" s="55"/>
-      <c r="B76" s="55"/>
+      <c r="A76" s="58"/>
+      <c r="B76" s="58"/>
       <c r="C76" s="8" t="s">
         <v>143</v>
       </c>
@@ -26916,8 +26920,8 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="50" customHeight="1">
-      <c r="A77" s="55"/>
-      <c r="B77" s="55"/>
+      <c r="A77" s="58"/>
+      <c r="B77" s="58"/>
       <c r="C77" s="8" t="s">
         <v>145</v>
       </c>
@@ -26936,8 +26940,8 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="50" customHeight="1">
-      <c r="A78" s="55"/>
-      <c r="B78" s="55"/>
+      <c r="A78" s="58"/>
+      <c r="B78" s="58"/>
       <c r="C78" s="8" t="s">
         <v>147</v>
       </c>
@@ -26956,8 +26960,8 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="50" customHeight="1">
-      <c r="A79" s="55"/>
-      <c r="B79" s="55"/>
+      <c r="A79" s="58"/>
+      <c r="B79" s="58"/>
       <c r="C79" s="8" t="s">
         <v>149</v>
       </c>
@@ -26976,8 +26980,8 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="50" customHeight="1">
-      <c r="A80" s="55"/>
-      <c r="B80" s="55"/>
+      <c r="A80" s="58"/>
+      <c r="B80" s="58"/>
       <c r="C80" s="8" t="s">
         <v>151</v>
       </c>
@@ -26996,8 +27000,8 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="50" customHeight="1">
-      <c r="A81" s="55"/>
-      <c r="B81" s="55"/>
+      <c r="A81" s="58"/>
+      <c r="B81" s="58"/>
       <c r="C81" s="8" t="s">
         <v>153</v>
       </c>
@@ -27016,8 +27020,8 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="50" customHeight="1">
-      <c r="A82" s="55"/>
-      <c r="B82" s="55"/>
+      <c r="A82" s="58"/>
+      <c r="B82" s="58"/>
       <c r="C82" s="8" t="s">
         <v>155</v>
       </c>
@@ -27036,8 +27040,8 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="50" customHeight="1">
-      <c r="A83" s="55"/>
-      <c r="B83" s="55"/>
+      <c r="A83" s="58"/>
+      <c r="B83" s="58"/>
       <c r="C83" s="8" t="s">
         <v>157</v>
       </c>
@@ -27056,8 +27060,8 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="50" customHeight="1">
-      <c r="A84" s="55"/>
-      <c r="B84" s="55"/>
+      <c r="A84" s="58"/>
+      <c r="B84" s="58"/>
       <c r="C84" s="8" t="s">
         <v>159</v>
       </c>
@@ -27076,8 +27080,8 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="50" customHeight="1">
-      <c r="A85" s="55"/>
-      <c r="B85" s="55"/>
+      <c r="A85" s="58"/>
+      <c r="B85" s="58"/>
       <c r="C85" s="8" t="s">
         <v>161</v>
       </c>
@@ -27096,8 +27100,8 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="50" customHeight="1">
-      <c r="A86" s="55"/>
-      <c r="B86" s="55"/>
+      <c r="A86" s="58"/>
+      <c r="B86" s="58"/>
       <c r="C86" s="8" t="s">
         <v>163</v>
       </c>
@@ -27116,8 +27120,8 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="50" customHeight="1">
-      <c r="A87" s="55"/>
-      <c r="B87" s="55"/>
+      <c r="A87" s="58"/>
+      <c r="B87" s="58"/>
       <c r="C87" s="8" t="s">
         <v>165</v>
       </c>
@@ -27136,8 +27140,8 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="50" customHeight="1">
-      <c r="A88" s="55"/>
-      <c r="B88" s="55"/>
+      <c r="A88" s="58"/>
+      <c r="B88" s="58"/>
       <c r="C88" s="8" t="s">
         <v>167</v>
       </c>
@@ -27156,8 +27160,8 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="50" customHeight="1">
-      <c r="A89" s="55"/>
-      <c r="B89" s="55"/>
+      <c r="A89" s="58"/>
+      <c r="B89" s="58"/>
       <c r="C89" s="8" t="s">
         <v>169</v>
       </c>
@@ -27176,8 +27180,8 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="50" customHeight="1">
-      <c r="A90" s="55"/>
-      <c r="B90" s="55"/>
+      <c r="A90" s="58"/>
+      <c r="B90" s="58"/>
       <c r="C90" s="8" t="s">
         <v>171</v>
       </c>
@@ -27196,8 +27200,8 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="50" customHeight="1">
-      <c r="A91" s="55"/>
-      <c r="B91" s="55"/>
+      <c r="A91" s="58"/>
+      <c r="B91" s="58"/>
       <c r="C91" s="8" t="s">
         <v>173</v>
       </c>
@@ -27216,8 +27220,8 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="50" customHeight="1">
-      <c r="A92" s="55"/>
-      <c r="B92" s="55"/>
+      <c r="A92" s="58"/>
+      <c r="B92" s="58"/>
       <c r="C92" s="8" t="s">
         <v>175</v>
       </c>
@@ -27236,8 +27240,8 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="50" customHeight="1">
-      <c r="A93" s="55"/>
-      <c r="B93" s="55"/>
+      <c r="A93" s="58"/>
+      <c r="B93" s="58"/>
       <c r="C93" s="8" t="s">
         <v>177</v>
       </c>
@@ -27256,8 +27260,8 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="50" customHeight="1">
-      <c r="A94" s="55"/>
-      <c r="B94" s="55"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="58"/>
       <c r="C94" s="8" t="s">
         <v>179</v>
       </c>
@@ -27276,8 +27280,8 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="50" customHeight="1">
-      <c r="A95" s="55"/>
-      <c r="B95" s="55"/>
+      <c r="A95" s="58"/>
+      <c r="B95" s="58"/>
       <c r="C95" s="8" t="s">
         <v>181</v>
       </c>
@@ -27296,8 +27300,8 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="50" customHeight="1">
-      <c r="A96" s="55"/>
-      <c r="B96" s="56"/>
+      <c r="A96" s="58"/>
+      <c r="B96" s="59"/>
       <c r="C96" s="8" t="s">
         <v>183</v>
       </c>
@@ -27316,8 +27320,8 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="50" customHeight="1">
-      <c r="A97" s="55"/>
-      <c r="B97" s="54" t="s">
+      <c r="A97" s="58"/>
+      <c r="B97" s="57" t="s">
         <v>851</v>
       </c>
       <c r="C97" s="8" t="s">
@@ -27338,8 +27342,8 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="50" customHeight="1">
-      <c r="A98" s="55"/>
-      <c r="B98" s="55"/>
+      <c r="A98" s="58"/>
+      <c r="B98" s="58"/>
       <c r="C98" s="8" t="s">
         <v>187</v>
       </c>
@@ -27358,8 +27362,8 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="50" customHeight="1">
-      <c r="A99" s="55"/>
-      <c r="B99" s="55"/>
+      <c r="A99" s="58"/>
+      <c r="B99" s="58"/>
       <c r="C99" s="8" t="s">
         <v>189</v>
       </c>
@@ -27378,8 +27382,8 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="50" customHeight="1">
-      <c r="A100" s="55"/>
-      <c r="B100" s="55"/>
+      <c r="A100" s="58"/>
+      <c r="B100" s="58"/>
       <c r="C100" s="8" t="s">
         <v>191</v>
       </c>
@@ -27390,16 +27394,16 @@
         <v>931</v>
       </c>
       <c r="F100" s="10"/>
-      <c r="G100" s="21" t="s">
-        <v>996</v>
-      </c>
-      <c r="H100" s="44" t="s">
-        <v>997</v>
+      <c r="G100" s="42" t="s">
+        <v>994</v>
+      </c>
+      <c r="H100" s="43" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="50" customHeight="1">
-      <c r="A101" s="55"/>
-      <c r="B101" s="55"/>
+      <c r="A101" s="58"/>
+      <c r="B101" s="58"/>
       <c r="C101" s="8" t="s">
         <v>193</v>
       </c>
@@ -27418,8 +27422,8 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="50" customHeight="1">
-      <c r="A102" s="55"/>
-      <c r="B102" s="55"/>
+      <c r="A102" s="58"/>
+      <c r="B102" s="58"/>
       <c r="C102" s="8" t="s">
         <v>195</v>
       </c>
@@ -27438,8 +27442,8 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="50" customHeight="1">
-      <c r="A103" s="55"/>
-      <c r="B103" s="55"/>
+      <c r="A103" s="58"/>
+      <c r="B103" s="58"/>
       <c r="C103" s="8" t="s">
         <v>197</v>
       </c>
@@ -27458,8 +27462,8 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="50" customHeight="1">
-      <c r="A104" s="55"/>
-      <c r="B104" s="55"/>
+      <c r="A104" s="58"/>
+      <c r="B104" s="58"/>
       <c r="C104" s="8" t="s">
         <v>199</v>
       </c>
@@ -27478,8 +27482,8 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="50" customHeight="1">
-      <c r="A105" s="55"/>
-      <c r="B105" s="55"/>
+      <c r="A105" s="58"/>
+      <c r="B105" s="58"/>
       <c r="C105" s="8" t="s">
         <v>201</v>
       </c>
@@ -27498,8 +27502,8 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="50" customHeight="1">
-      <c r="A106" s="55"/>
-      <c r="B106" s="56"/>
+      <c r="A106" s="58"/>
+      <c r="B106" s="59"/>
       <c r="C106" s="8" t="s">
         <v>203</v>
       </c>
@@ -27518,8 +27522,8 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="50" customHeight="1">
-      <c r="A107" s="55"/>
-      <c r="B107" s="54" t="s">
+      <c r="A107" s="58"/>
+      <c r="B107" s="57" t="s">
         <v>852</v>
       </c>
       <c r="C107" s="8" t="s">
@@ -27540,8 +27544,8 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="50" customHeight="1">
-      <c r="A108" s="55"/>
-      <c r="B108" s="55"/>
+      <c r="A108" s="58"/>
+      <c r="B108" s="58"/>
       <c r="C108" s="8" t="s">
         <v>207</v>
       </c>
@@ -27560,8 +27564,8 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="50" customHeight="1">
-      <c r="A109" s="55"/>
-      <c r="B109" s="55"/>
+      <c r="A109" s="58"/>
+      <c r="B109" s="58"/>
       <c r="C109" s="8" t="s">
         <v>209</v>
       </c>
@@ -27580,8 +27584,8 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="50" customHeight="1">
-      <c r="A110" s="55"/>
-      <c r="B110" s="55"/>
+      <c r="A110" s="58"/>
+      <c r="B110" s="58"/>
       <c r="C110" s="8" t="s">
         <v>211</v>
       </c>
@@ -27600,8 +27604,8 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="50" customHeight="1">
-      <c r="A111" s="55"/>
-      <c r="B111" s="55"/>
+      <c r="A111" s="58"/>
+      <c r="B111" s="58"/>
       <c r="C111" s="8" t="s">
         <v>213</v>
       </c>
@@ -27620,8 +27624,8 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="50" customHeight="1">
-      <c r="A112" s="56"/>
-      <c r="B112" s="56"/>
+      <c r="A112" s="59"/>
+      <c r="B112" s="59"/>
       <c r="C112" s="8" t="s">
         <v>215</v>
       </c>
@@ -27632,18 +27636,18 @@
         <v>964</v>
       </c>
       <c r="F112" s="10"/>
-      <c r="G112" s="20" t="s">
-        <v>998</v>
-      </c>
-      <c r="H112" s="45" t="s">
-        <v>999</v>
+      <c r="G112" s="23" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H112" s="47" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="50" customHeight="1">
-      <c r="A113" s="54" t="s">
+      <c r="A113" s="57" t="s">
         <v>853</v>
       </c>
-      <c r="B113" s="54" t="s">
+      <c r="B113" s="57" t="s">
         <v>854</v>
       </c>
       <c r="C113" s="8" t="s">
@@ -27664,8 +27668,8 @@
       </c>
     </row>
     <row r="114" spans="1:8" ht="50" customHeight="1">
-      <c r="A114" s="55"/>
-      <c r="B114" s="55"/>
+      <c r="A114" s="58"/>
+      <c r="B114" s="58"/>
       <c r="C114" s="8" t="s">
         <v>219</v>
       </c>
@@ -27684,8 +27688,8 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="50" customHeight="1">
-      <c r="A115" s="55"/>
-      <c r="B115" s="56"/>
+      <c r="A115" s="58"/>
+      <c r="B115" s="59"/>
       <c r="C115" s="8" t="s">
         <v>221</v>
       </c>
@@ -27704,8 +27708,8 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="50" customHeight="1">
-      <c r="A116" s="55"/>
-      <c r="B116" s="60" t="s">
+      <c r="A116" s="58"/>
+      <c r="B116" s="54" t="s">
         <v>855</v>
       </c>
       <c r="C116" s="8" t="s">
@@ -27726,8 +27730,8 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="50" customHeight="1">
-      <c r="A117" s="55"/>
-      <c r="B117" s="61"/>
+      <c r="A117" s="58"/>
+      <c r="B117" s="55"/>
       <c r="C117" s="8" t="s">
         <v>225</v>
       </c>
@@ -27746,8 +27750,8 @@
       </c>
     </row>
     <row r="118" spans="1:8" ht="50" customHeight="1">
-      <c r="A118" s="55"/>
-      <c r="B118" s="61"/>
+      <c r="A118" s="58"/>
+      <c r="B118" s="55"/>
       <c r="C118" s="8" t="s">
         <v>227</v>
       </c>
@@ -27766,8 +27770,8 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="50" customHeight="1">
-      <c r="A119" s="55"/>
-      <c r="B119" s="61"/>
+      <c r="A119" s="58"/>
+      <c r="B119" s="55"/>
       <c r="C119" s="8" t="s">
         <v>229</v>
       </c>
@@ -27786,8 +27790,8 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="50" customHeight="1">
-      <c r="A120" s="55"/>
-      <c r="B120" s="61"/>
+      <c r="A120" s="58"/>
+      <c r="B120" s="55"/>
       <c r="C120" s="8" t="s">
         <v>231</v>
       </c>
@@ -27806,8 +27810,8 @@
       </c>
     </row>
     <row r="121" spans="1:8" ht="50" customHeight="1">
-      <c r="A121" s="55"/>
-      <c r="B121" s="61"/>
+      <c r="A121" s="58"/>
+      <c r="B121" s="55"/>
       <c r="C121" s="8" t="s">
         <v>233</v>
       </c>
@@ -27826,8 +27830,8 @@
       </c>
     </row>
     <row r="122" spans="1:8" ht="50" customHeight="1">
-      <c r="A122" s="55"/>
-      <c r="B122" s="61"/>
+      <c r="A122" s="58"/>
+      <c r="B122" s="55"/>
       <c r="C122" s="8" t="s">
         <v>235</v>
       </c>
@@ -27847,7 +27851,7 @@
     </row>
     <row r="123" spans="1:8" ht="50" customHeight="1">
       <c r="A123" s="17"/>
-      <c r="B123" s="61"/>
+      <c r="B123" s="55"/>
       <c r="C123" s="35" t="s">
         <v>903</v>
       </c>
@@ -27866,10 +27870,10 @@
       </c>
     </row>
     <row r="124" spans="1:8" ht="50" customHeight="1">
-      <c r="A124" s="55" t="s">
+      <c r="A124" s="58" t="s">
         <v>856</v>
       </c>
-      <c r="B124" s="55" t="s">
+      <c r="B124" s="58" t="s">
         <v>857</v>
       </c>
       <c r="C124" s="8" t="s">
@@ -27890,8 +27894,8 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="50" customHeight="1">
-      <c r="A125" s="55"/>
-      <c r="B125" s="55"/>
+      <c r="A125" s="58"/>
+      <c r="B125" s="58"/>
       <c r="C125" s="8" t="s">
         <v>239</v>
       </c>
@@ -27910,8 +27914,8 @@
       </c>
     </row>
     <row r="126" spans="1:8" ht="50" customHeight="1">
-      <c r="A126" s="55"/>
-      <c r="B126" s="55"/>
+      <c r="A126" s="58"/>
+      <c r="B126" s="58"/>
       <c r="C126" s="8" t="s">
         <v>241</v>
       </c>
@@ -27930,8 +27934,8 @@
       </c>
     </row>
     <row r="127" spans="1:8" ht="50" customHeight="1">
-      <c r="A127" s="55"/>
-      <c r="B127" s="55"/>
+      <c r="A127" s="58"/>
+      <c r="B127" s="58"/>
       <c r="C127" s="8" t="s">
         <v>243</v>
       </c>
@@ -27950,8 +27954,8 @@
       </c>
     </row>
     <row r="128" spans="1:8" ht="50" customHeight="1">
-      <c r="A128" s="55"/>
-      <c r="B128" s="55"/>
+      <c r="A128" s="58"/>
+      <c r="B128" s="58"/>
       <c r="C128" s="8" t="s">
         <v>245</v>
       </c>
@@ -27970,8 +27974,8 @@
       </c>
     </row>
     <row r="129" spans="1:8" ht="50" customHeight="1">
-      <c r="A129" s="55"/>
-      <c r="B129" s="55"/>
+      <c r="A129" s="58"/>
+      <c r="B129" s="58"/>
       <c r="C129" s="8" t="s">
         <v>247</v>
       </c>
@@ -27990,8 +27994,8 @@
       </c>
     </row>
     <row r="130" spans="1:8" ht="50" customHeight="1">
-      <c r="A130" s="55"/>
-      <c r="B130" s="55"/>
+      <c r="A130" s="58"/>
+      <c r="B130" s="58"/>
       <c r="C130" s="8" t="s">
         <v>249</v>
       </c>
@@ -28010,8 +28014,8 @@
       </c>
     </row>
     <row r="131" spans="1:8" ht="50" customHeight="1">
-      <c r="A131" s="55"/>
-      <c r="B131" s="55"/>
+      <c r="A131" s="58"/>
+      <c r="B131" s="58"/>
       <c r="C131" s="8" t="s">
         <v>251</v>
       </c>
@@ -28030,8 +28034,8 @@
       </c>
     </row>
     <row r="132" spans="1:8" ht="50" customHeight="1">
-      <c r="A132" s="55"/>
-      <c r="B132" s="55"/>
+      <c r="A132" s="58"/>
+      <c r="B132" s="58"/>
       <c r="C132" s="8" t="s">
         <v>253</v>
       </c>
@@ -28050,8 +28054,8 @@
       </c>
     </row>
     <row r="133" spans="1:8" ht="50" customHeight="1">
-      <c r="A133" s="55"/>
-      <c r="B133" s="55"/>
+      <c r="A133" s="58"/>
+      <c r="B133" s="58"/>
       <c r="C133" s="8" t="s">
         <v>255</v>
       </c>
@@ -28070,8 +28074,8 @@
       </c>
     </row>
     <row r="134" spans="1:8" ht="50" customHeight="1">
-      <c r="A134" s="55"/>
-      <c r="B134" s="55"/>
+      <c r="A134" s="58"/>
+      <c r="B134" s="58"/>
       <c r="C134" s="8" t="s">
         <v>257</v>
       </c>
@@ -28090,8 +28094,8 @@
       </c>
     </row>
     <row r="135" spans="1:8" ht="50" customHeight="1">
-      <c r="A135" s="55"/>
-      <c r="B135" s="55"/>
+      <c r="A135" s="58"/>
+      <c r="B135" s="58"/>
       <c r="C135" s="8" t="s">
         <v>259</v>
       </c>
@@ -28102,16 +28106,16 @@
         <v>933</v>
       </c>
       <c r="F135" s="10"/>
-      <c r="G135" s="23" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H135" s="47" t="s">
-        <v>1003</v>
+      <c r="G135" s="22" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H135" s="46" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="50" customHeight="1">
-      <c r="A136" s="55"/>
-      <c r="B136" s="55"/>
+      <c r="A136" s="58"/>
+      <c r="B136" s="58"/>
       <c r="C136" s="8" t="s">
         <v>261</v>
       </c>
@@ -28130,8 +28134,8 @@
       </c>
     </row>
     <row r="137" spans="1:8" ht="50" customHeight="1">
-      <c r="A137" s="55"/>
-      <c r="B137" s="55"/>
+      <c r="A137" s="58"/>
+      <c r="B137" s="58"/>
       <c r="C137" s="8" t="s">
         <v>263</v>
       </c>
@@ -28150,8 +28154,8 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="50" customHeight="1">
-      <c r="A138" s="55"/>
-      <c r="B138" s="56"/>
+      <c r="A138" s="58"/>
+      <c r="B138" s="59"/>
       <c r="C138" s="8" t="s">
         <v>265</v>
       </c>
@@ -28170,8 +28174,8 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="50" customHeight="1">
-      <c r="A139" s="55"/>
-      <c r="B139" s="54" t="s">
+      <c r="A139" s="58"/>
+      <c r="B139" s="57" t="s">
         <v>858</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -28192,8 +28196,8 @@
       </c>
     </row>
     <row r="140" spans="1:8" ht="50" customHeight="1">
-      <c r="A140" s="55"/>
-      <c r="B140" s="55"/>
+      <c r="A140" s="58"/>
+      <c r="B140" s="58"/>
       <c r="C140" s="8" t="s">
         <v>269</v>
       </c>
@@ -28212,8 +28216,8 @@
       </c>
     </row>
     <row r="141" spans="1:8" ht="50" customHeight="1">
-      <c r="A141" s="55"/>
-      <c r="B141" s="55"/>
+      <c r="A141" s="58"/>
+      <c r="B141" s="58"/>
       <c r="C141" s="8" t="s">
         <v>271</v>
       </c>
@@ -28232,8 +28236,8 @@
       </c>
     </row>
     <row r="142" spans="1:8" ht="50" customHeight="1">
-      <c r="A142" s="55"/>
-      <c r="B142" s="55"/>
+      <c r="A142" s="58"/>
+      <c r="B142" s="58"/>
       <c r="C142" s="8" t="s">
         <v>273</v>
       </c>
@@ -28252,8 +28256,8 @@
       </c>
     </row>
     <row r="143" spans="1:8" ht="50" customHeight="1">
-      <c r="A143" s="55"/>
-      <c r="B143" s="55"/>
+      <c r="A143" s="58"/>
+      <c r="B143" s="58"/>
       <c r="C143" s="8" t="s">
         <v>275</v>
       </c>
@@ -28272,8 +28276,8 @@
       </c>
     </row>
     <row r="144" spans="1:8" ht="50" customHeight="1">
-      <c r="A144" s="55"/>
-      <c r="B144" s="55"/>
+      <c r="A144" s="58"/>
+      <c r="B144" s="58"/>
       <c r="C144" s="8" t="s">
         <v>277</v>
       </c>
@@ -28284,16 +28288,16 @@
         <v>930</v>
       </c>
       <c r="F144" s="10"/>
-      <c r="G144" s="23" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H144" s="47" t="s">
-        <v>1003</v>
+      <c r="G144" s="18" t="s">
+        <v>990</v>
+      </c>
+      <c r="H144" s="40" t="s">
+        <v>991</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="50" customHeight="1">
-      <c r="A145" s="55"/>
-      <c r="B145" s="55"/>
+      <c r="A145" s="58"/>
+      <c r="B145" s="58"/>
       <c r="C145" s="8" t="s">
         <v>279</v>
       </c>
@@ -28312,8 +28316,8 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="50" customHeight="1">
-      <c r="A146" s="55"/>
-      <c r="B146" s="55"/>
+      <c r="A146" s="58"/>
+      <c r="B146" s="58"/>
       <c r="C146" s="8" t="s">
         <v>281</v>
       </c>
@@ -28332,8 +28336,8 @@
       </c>
     </row>
     <row r="147" spans="1:8" ht="50" customHeight="1">
-      <c r="A147" s="56"/>
-      <c r="B147" s="56"/>
+      <c r="A147" s="59"/>
+      <c r="B147" s="59"/>
       <c r="C147" s="8" t="s">
         <v>283</v>
       </c>
@@ -28351,7 +28355,7 @@
       </c>
     </row>
     <row r="148" spans="1:8" ht="50" customHeight="1">
-      <c r="A148" s="54" t="s">
+      <c r="A148" s="57" t="s">
         <v>859</v>
       </c>
       <c r="B148" s="14" t="s">
@@ -28375,7 +28379,7 @@
       </c>
     </row>
     <row r="149" spans="1:8" ht="50" customHeight="1">
-      <c r="A149" s="55"/>
+      <c r="A149" s="58"/>
       <c r="B149" s="14" t="s">
         <v>868</v>
       </c>
@@ -28397,7 +28401,7 @@
       </c>
     </row>
     <row r="150" spans="1:8" ht="50" customHeight="1">
-      <c r="A150" s="55"/>
+      <c r="A150" s="58"/>
       <c r="B150" s="14" t="s">
         <v>869</v>
       </c>
@@ -28419,8 +28423,8 @@
       </c>
     </row>
     <row r="151" spans="1:8" ht="50" customHeight="1">
-      <c r="A151" s="55"/>
-      <c r="B151" s="57" t="s">
+      <c r="A151" s="58"/>
+      <c r="B151" s="62" t="s">
         <v>870</v>
       </c>
       <c r="C151" s="8" t="s">
@@ -28441,8 +28445,8 @@
       </c>
     </row>
     <row r="152" spans="1:8" ht="50" customHeight="1">
-      <c r="A152" s="55"/>
-      <c r="B152" s="58"/>
+      <c r="A152" s="58"/>
+      <c r="B152" s="63"/>
       <c r="C152" s="8" t="s">
         <v>293</v>
       </c>
@@ -28461,8 +28465,8 @@
       </c>
     </row>
     <row r="153" spans="1:8" ht="50" customHeight="1">
-      <c r="A153" s="55"/>
-      <c r="B153" s="58"/>
+      <c r="A153" s="58"/>
+      <c r="B153" s="63"/>
       <c r="C153" s="8" t="s">
         <v>295</v>
       </c>
@@ -28481,8 +28485,8 @@
       </c>
     </row>
     <row r="154" spans="1:8" ht="50" customHeight="1">
-      <c r="A154" s="55"/>
-      <c r="B154" s="58"/>
+      <c r="A154" s="58"/>
+      <c r="B154" s="63"/>
       <c r="C154" s="8" t="s">
         <v>297</v>
       </c>
@@ -28501,8 +28505,8 @@
       </c>
     </row>
     <row r="155" spans="1:8" ht="50" customHeight="1">
-      <c r="A155" s="55"/>
-      <c r="B155" s="58"/>
+      <c r="A155" s="58"/>
+      <c r="B155" s="63"/>
       <c r="C155" s="8" t="s">
         <v>299</v>
       </c>
@@ -28521,8 +28525,8 @@
       </c>
     </row>
     <row r="156" spans="1:8" ht="50" customHeight="1">
-      <c r="A156" s="55"/>
-      <c r="B156" s="58"/>
+      <c r="A156" s="58"/>
+      <c r="B156" s="63"/>
       <c r="C156" s="8" t="s">
         <v>301</v>
       </c>
@@ -28541,8 +28545,8 @@
       </c>
     </row>
     <row r="157" spans="1:8" ht="50" customHeight="1">
-      <c r="A157" s="55"/>
-      <c r="B157" s="58"/>
+      <c r="A157" s="58"/>
+      <c r="B157" s="63"/>
       <c r="C157" s="35" t="s">
         <v>901</v>
       </c>
@@ -28561,8 +28565,8 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="50" customHeight="1">
-      <c r="A158" s="55"/>
-      <c r="B158" s="58"/>
+      <c r="A158" s="58"/>
+      <c r="B158" s="63"/>
       <c r="C158" s="8" t="s">
         <v>303</v>
       </c>
@@ -28581,8 +28585,8 @@
       </c>
     </row>
     <row r="159" spans="1:8" ht="50" customHeight="1">
-      <c r="A159" s="55"/>
-      <c r="B159" s="59"/>
+      <c r="A159" s="58"/>
+      <c r="B159" s="64"/>
       <c r="C159" s="8" t="s">
         <v>305</v>
       </c>
@@ -28601,8 +28605,8 @@
       </c>
     </row>
     <row r="160" spans="1:8" ht="50" customHeight="1">
-      <c r="A160" s="55"/>
-      <c r="B160" s="54" t="s">
+      <c r="A160" s="58"/>
+      <c r="B160" s="57" t="s">
         <v>871</v>
       </c>
       <c r="C160" s="8" t="s">
@@ -28615,16 +28619,16 @@
         <v>936</v>
       </c>
       <c r="F160" s="10"/>
-      <c r="G160" s="29" t="s">
-        <v>1004</v>
-      </c>
-      <c r="H160" s="48" t="s">
-        <v>1005</v>
+      <c r="G160" s="30" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H160" s="49" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="50" customHeight="1">
-      <c r="A161" s="55"/>
-      <c r="B161" s="55"/>
+      <c r="A161" s="58"/>
+      <c r="B161" s="58"/>
       <c r="C161" s="8" t="s">
         <v>309</v>
       </c>
@@ -28643,8 +28647,8 @@
       </c>
     </row>
     <row r="162" spans="1:8" ht="50" customHeight="1">
-      <c r="A162" s="55"/>
-      <c r="B162" s="56"/>
+      <c r="A162" s="58"/>
+      <c r="B162" s="59"/>
       <c r="C162" s="8" t="s">
         <v>311</v>
       </c>
@@ -28663,8 +28667,8 @@
       </c>
     </row>
     <row r="163" spans="1:8" ht="50" customHeight="1">
-      <c r="A163" s="55"/>
-      <c r="B163" s="54" t="s">
+      <c r="A163" s="58"/>
+      <c r="B163" s="57" t="s">
         <v>872</v>
       </c>
       <c r="C163" s="8" t="s">
@@ -28685,8 +28689,8 @@
       </c>
     </row>
     <row r="164" spans="1:8" ht="50" customHeight="1">
-      <c r="A164" s="55"/>
-      <c r="B164" s="55"/>
+      <c r="A164" s="58"/>
+      <c r="B164" s="58"/>
       <c r="C164" s="8" t="s">
         <v>315</v>
       </c>
@@ -28705,8 +28709,8 @@
       </c>
     </row>
     <row r="165" spans="1:8" ht="50" customHeight="1">
-      <c r="A165" s="55"/>
-      <c r="B165" s="55"/>
+      <c r="A165" s="58"/>
+      <c r="B165" s="58"/>
       <c r="C165" s="8" t="s">
         <v>317</v>
       </c>
@@ -28725,8 +28729,8 @@
       </c>
     </row>
     <row r="166" spans="1:8" ht="50" customHeight="1">
-      <c r="A166" s="55"/>
-      <c r="B166" s="55"/>
+      <c r="A166" s="58"/>
+      <c r="B166" s="58"/>
       <c r="C166" s="8" t="s">
         <v>319</v>
       </c>
@@ -28745,8 +28749,8 @@
       </c>
     </row>
     <row r="167" spans="1:8" ht="50" customHeight="1">
-      <c r="A167" s="55"/>
-      <c r="B167" s="56"/>
+      <c r="A167" s="58"/>
+      <c r="B167" s="59"/>
       <c r="C167" s="13" t="s">
         <v>321</v>
       </c>
@@ -28764,8 +28768,8 @@
       </c>
     </row>
     <row r="168" spans="1:8" ht="50" customHeight="1">
-      <c r="A168" s="55"/>
-      <c r="B168" s="54" t="s">
+      <c r="A168" s="58"/>
+      <c r="B168" s="57" t="s">
         <v>873</v>
       </c>
       <c r="C168" s="8" t="s">
@@ -28786,8 +28790,8 @@
       </c>
     </row>
     <row r="169" spans="1:8" ht="50" customHeight="1">
-      <c r="A169" s="55"/>
-      <c r="B169" s="55"/>
+      <c r="A169" s="58"/>
+      <c r="B169" s="58"/>
       <c r="C169" s="8" t="s">
         <v>325</v>
       </c>
@@ -28806,8 +28810,8 @@
       </c>
     </row>
     <row r="170" spans="1:8" ht="50" customHeight="1">
-      <c r="A170" s="55"/>
-      <c r="B170" s="55"/>
+      <c r="A170" s="58"/>
+      <c r="B170" s="58"/>
       <c r="C170" s="8" t="s">
         <v>326</v>
       </c>
@@ -28826,8 +28830,8 @@
       </c>
     </row>
     <row r="171" spans="1:8" ht="50" customHeight="1">
-      <c r="A171" s="55"/>
-      <c r="B171" s="55"/>
+      <c r="A171" s="58"/>
+      <c r="B171" s="58"/>
       <c r="C171" s="8" t="s">
         <v>328</v>
       </c>
@@ -28846,8 +28850,8 @@
       </c>
     </row>
     <row r="172" spans="1:8" ht="50" customHeight="1">
-      <c r="A172" s="55"/>
-      <c r="B172" s="55"/>
+      <c r="A172" s="58"/>
+      <c r="B172" s="58"/>
       <c r="C172" s="8" t="s">
         <v>330</v>
       </c>
@@ -28866,8 +28870,8 @@
       </c>
     </row>
     <row r="173" spans="1:8" ht="50" customHeight="1">
-      <c r="A173" s="55"/>
-      <c r="B173" s="55"/>
+      <c r="A173" s="58"/>
+      <c r="B173" s="58"/>
       <c r="C173" s="8" t="s">
         <v>332</v>
       </c>
@@ -28886,8 +28890,8 @@
       </c>
     </row>
     <row r="174" spans="1:8" ht="50" customHeight="1">
-      <c r="A174" s="55"/>
-      <c r="B174" s="55"/>
+      <c r="A174" s="58"/>
+      <c r="B174" s="58"/>
       <c r="C174" s="8" t="s">
         <v>334</v>
       </c>
@@ -28906,8 +28910,8 @@
       </c>
     </row>
     <row r="175" spans="1:8" ht="50" customHeight="1">
-      <c r="A175" s="55"/>
-      <c r="B175" s="55"/>
+      <c r="A175" s="58"/>
+      <c r="B175" s="58"/>
       <c r="C175" s="8" t="s">
         <v>336</v>
       </c>
@@ -28926,8 +28930,8 @@
       </c>
     </row>
     <row r="176" spans="1:8" ht="50" customHeight="1">
-      <c r="A176" s="55"/>
-      <c r="B176" s="55"/>
+      <c r="A176" s="58"/>
+      <c r="B176" s="58"/>
       <c r="C176" s="8" t="s">
         <v>338</v>
       </c>
@@ -28946,8 +28950,8 @@
       </c>
     </row>
     <row r="177" spans="1:8" ht="50" customHeight="1">
-      <c r="A177" s="55"/>
-      <c r="B177" s="55"/>
+      <c r="A177" s="58"/>
+      <c r="B177" s="58"/>
       <c r="C177" s="8" t="s">
         <v>340</v>
       </c>
@@ -28966,8 +28970,8 @@
       </c>
     </row>
     <row r="178" spans="1:8" ht="50" customHeight="1">
-      <c r="A178" s="55"/>
-      <c r="B178" s="56"/>
+      <c r="A178" s="58"/>
+      <c r="B178" s="59"/>
       <c r="C178" s="8" t="s">
         <v>342</v>
       </c>
@@ -28986,8 +28990,8 @@
       </c>
     </row>
     <row r="179" spans="1:8" ht="50" customHeight="1">
-      <c r="A179" s="55"/>
-      <c r="B179" s="54" t="s">
+      <c r="A179" s="58"/>
+      <c r="B179" s="57" t="s">
         <v>874</v>
       </c>
       <c r="C179" s="8" t="s">
@@ -29008,8 +29012,8 @@
       </c>
     </row>
     <row r="180" spans="1:8" ht="50" customHeight="1">
-      <c r="A180" s="55"/>
-      <c r="B180" s="56"/>
+      <c r="A180" s="58"/>
+      <c r="B180" s="59"/>
       <c r="C180" s="8" t="s">
         <v>346</v>
       </c>
@@ -29028,8 +29032,8 @@
       </c>
     </row>
     <row r="181" spans="1:8" ht="50" customHeight="1">
-      <c r="A181" s="55"/>
-      <c r="B181" s="54" t="s">
+      <c r="A181" s="58"/>
+      <c r="B181" s="57" t="s">
         <v>875</v>
       </c>
       <c r="C181" s="8" t="s">
@@ -29050,8 +29054,8 @@
       </c>
     </row>
     <row r="182" spans="1:8" ht="50" customHeight="1">
-      <c r="A182" s="55"/>
-      <c r="B182" s="55"/>
+      <c r="A182" s="58"/>
+      <c r="B182" s="58"/>
       <c r="C182" s="8" t="s">
         <v>350</v>
       </c>
@@ -29070,8 +29074,8 @@
       </c>
     </row>
     <row r="183" spans="1:8" ht="50" customHeight="1">
-      <c r="A183" s="55"/>
-      <c r="B183" s="55"/>
+      <c r="A183" s="58"/>
+      <c r="B183" s="58"/>
       <c r="C183" s="8" t="s">
         <v>352</v>
       </c>
@@ -29090,8 +29094,8 @@
       </c>
     </row>
     <row r="184" spans="1:8" ht="50" customHeight="1">
-      <c r="A184" s="55"/>
-      <c r="B184" s="55"/>
+      <c r="A184" s="58"/>
+      <c r="B184" s="58"/>
       <c r="C184" s="8" t="s">
         <v>354</v>
       </c>
@@ -29110,8 +29114,8 @@
       </c>
     </row>
     <row r="185" spans="1:8" ht="50" customHeight="1">
-      <c r="A185" s="55"/>
-      <c r="B185" s="55"/>
+      <c r="A185" s="58"/>
+      <c r="B185" s="58"/>
       <c r="C185" s="8" t="s">
         <v>356</v>
       </c>
@@ -29130,8 +29134,8 @@
       </c>
     </row>
     <row r="186" spans="1:8" ht="50" customHeight="1">
-      <c r="A186" s="55"/>
-      <c r="B186" s="56"/>
+      <c r="A186" s="58"/>
+      <c r="B186" s="59"/>
       <c r="C186" s="8" t="s">
         <v>358</v>
       </c>
@@ -29150,8 +29154,8 @@
       </c>
     </row>
     <row r="187" spans="1:8" ht="50" customHeight="1">
-      <c r="A187" s="55"/>
-      <c r="B187" s="54" t="s">
+      <c r="A187" s="58"/>
+      <c r="B187" s="57" t="s">
         <v>876</v>
       </c>
       <c r="C187" s="8" t="s">
@@ -29172,8 +29176,8 @@
       </c>
     </row>
     <row r="188" spans="1:8" ht="50" customHeight="1">
-      <c r="A188" s="55"/>
-      <c r="B188" s="55"/>
+      <c r="A188" s="58"/>
+      <c r="B188" s="58"/>
       <c r="C188" s="8" t="s">
         <v>362</v>
       </c>
@@ -29192,8 +29196,8 @@
       </c>
     </row>
     <row r="189" spans="1:8" ht="50" customHeight="1">
-      <c r="A189" s="55"/>
-      <c r="B189" s="55"/>
+      <c r="A189" s="58"/>
+      <c r="B189" s="58"/>
       <c r="C189" s="8" t="s">
         <v>364</v>
       </c>
@@ -29212,8 +29216,8 @@
       </c>
     </row>
     <row r="190" spans="1:8" ht="50" customHeight="1">
-      <c r="A190" s="55"/>
-      <c r="B190" s="55"/>
+      <c r="A190" s="58"/>
+      <c r="B190" s="58"/>
       <c r="C190" s="8" t="s">
         <v>366</v>
       </c>
@@ -29232,8 +29236,8 @@
       </c>
     </row>
     <row r="191" spans="1:8" ht="50" customHeight="1">
-      <c r="A191" s="55"/>
-      <c r="B191" s="55"/>
+      <c r="A191" s="58"/>
+      <c r="B191" s="58"/>
       <c r="C191" s="8" t="s">
         <v>368</v>
       </c>
@@ -29252,8 +29256,8 @@
       </c>
     </row>
     <row r="192" spans="1:8" ht="50" customHeight="1">
-      <c r="A192" s="55"/>
-      <c r="B192" s="55"/>
+      <c r="A192" s="58"/>
+      <c r="B192" s="58"/>
       <c r="C192" s="8" t="s">
         <v>370</v>
       </c>
@@ -29272,8 +29276,8 @@
       </c>
     </row>
     <row r="193" spans="1:8" ht="50" customHeight="1">
-      <c r="A193" s="55"/>
-      <c r="B193" s="55"/>
+      <c r="A193" s="58"/>
+      <c r="B193" s="58"/>
       <c r="C193" s="8" t="s">
         <v>372</v>
       </c>
@@ -29292,8 +29296,8 @@
       </c>
     </row>
     <row r="194" spans="1:8" ht="50" customHeight="1">
-      <c r="A194" s="55"/>
-      <c r="B194" s="55"/>
+      <c r="A194" s="58"/>
+      <c r="B194" s="58"/>
       <c r="C194" s="8" t="s">
         <v>374</v>
       </c>
@@ -29312,8 +29316,8 @@
       </c>
     </row>
     <row r="195" spans="1:8" ht="50" customHeight="1">
-      <c r="A195" s="55"/>
-      <c r="B195" s="55"/>
+      <c r="A195" s="58"/>
+      <c r="B195" s="58"/>
       <c r="C195" s="8" t="s">
         <v>376</v>
       </c>
@@ -29332,8 +29336,8 @@
       </c>
     </row>
     <row r="196" spans="1:8" ht="50" customHeight="1">
-      <c r="A196" s="55"/>
-      <c r="B196" s="55"/>
+      <c r="A196" s="58"/>
+      <c r="B196" s="58"/>
       <c r="C196" s="8" t="s">
         <v>378</v>
       </c>
@@ -29352,8 +29356,8 @@
       </c>
     </row>
     <row r="197" spans="1:8" ht="50" customHeight="1">
-      <c r="A197" s="55"/>
-      <c r="B197" s="55"/>
+      <c r="A197" s="58"/>
+      <c r="B197" s="58"/>
       <c r="C197" s="8" t="s">
         <v>380</v>
       </c>
@@ -29372,8 +29376,8 @@
       </c>
     </row>
     <row r="198" spans="1:8" ht="50" customHeight="1">
-      <c r="A198" s="55"/>
-      <c r="B198" s="55"/>
+      <c r="A198" s="58"/>
+      <c r="B198" s="58"/>
       <c r="C198" s="8" t="s">
         <v>382</v>
       </c>
@@ -29392,8 +29396,8 @@
       </c>
     </row>
     <row r="199" spans="1:8" ht="50" customHeight="1">
-      <c r="A199" s="55"/>
-      <c r="B199" s="55"/>
+      <c r="A199" s="58"/>
+      <c r="B199" s="58"/>
       <c r="C199" s="8" t="s">
         <v>384</v>
       </c>
@@ -29412,8 +29416,8 @@
       </c>
     </row>
     <row r="200" spans="1:8" ht="50" customHeight="1">
-      <c r="A200" s="55"/>
-      <c r="B200" s="55"/>
+      <c r="A200" s="58"/>
+      <c r="B200" s="58"/>
       <c r="C200" s="35" t="s">
         <v>897</v>
       </c>
@@ -29432,8 +29436,8 @@
       </c>
     </row>
     <row r="201" spans="1:8" ht="50" customHeight="1">
-      <c r="A201" s="55"/>
-      <c r="B201" s="55"/>
+      <c r="A201" s="58"/>
+      <c r="B201" s="58"/>
       <c r="C201" s="35" t="s">
         <v>899</v>
       </c>
@@ -29452,8 +29456,8 @@
       </c>
     </row>
     <row r="202" spans="1:8" ht="50" customHeight="1">
-      <c r="A202" s="55"/>
-      <c r="B202" s="55"/>
+      <c r="A202" s="58"/>
+      <c r="B202" s="58"/>
       <c r="C202" s="8" t="s">
         <v>386</v>
       </c>
@@ -29472,8 +29476,8 @@
       </c>
     </row>
     <row r="203" spans="1:8" ht="50" customHeight="1">
-      <c r="A203" s="55"/>
-      <c r="B203" s="55"/>
+      <c r="A203" s="58"/>
+      <c r="B203" s="58"/>
       <c r="C203" s="8" t="s">
         <v>388</v>
       </c>
@@ -29492,8 +29496,8 @@
       </c>
     </row>
     <row r="204" spans="1:8" ht="50" customHeight="1">
-      <c r="A204" s="55"/>
-      <c r="B204" s="55"/>
+      <c r="A204" s="58"/>
+      <c r="B204" s="58"/>
       <c r="C204" s="8" t="s">
         <v>390</v>
       </c>
@@ -29512,8 +29516,8 @@
       </c>
     </row>
     <row r="205" spans="1:8" ht="50" customHeight="1">
-      <c r="A205" s="55"/>
-      <c r="B205" s="55"/>
+      <c r="A205" s="58"/>
+      <c r="B205" s="58"/>
       <c r="C205" s="8" t="s">
         <v>392</v>
       </c>
@@ -29532,8 +29536,8 @@
       </c>
     </row>
     <row r="206" spans="1:8" ht="50" customHeight="1">
-      <c r="A206" s="55"/>
-      <c r="B206" s="55"/>
+      <c r="A206" s="58"/>
+      <c r="B206" s="58"/>
       <c r="C206" s="8" t="s">
         <v>394</v>
       </c>
@@ -29552,8 +29556,8 @@
       </c>
     </row>
     <row r="207" spans="1:8" ht="50" customHeight="1">
-      <c r="A207" s="55"/>
-      <c r="B207" s="55"/>
+      <c r="A207" s="58"/>
+      <c r="B207" s="58"/>
       <c r="C207" s="8" t="s">
         <v>396</v>
       </c>
@@ -29572,8 +29576,8 @@
       </c>
     </row>
     <row r="208" spans="1:8" ht="50" customHeight="1">
-      <c r="A208" s="55"/>
-      <c r="B208" s="55"/>
+      <c r="A208" s="58"/>
+      <c r="B208" s="58"/>
       <c r="C208" s="8" t="s">
         <v>398</v>
       </c>
@@ -29592,8 +29596,8 @@
       </c>
     </row>
     <row r="209" spans="1:8" ht="50" customHeight="1">
-      <c r="A209" s="55"/>
-      <c r="B209" s="55"/>
+      <c r="A209" s="58"/>
+      <c r="B209" s="58"/>
       <c r="C209" s="8" t="s">
         <v>400</v>
       </c>
@@ -29612,8 +29616,8 @@
       </c>
     </row>
     <row r="210" spans="1:8" ht="50" customHeight="1">
-      <c r="A210" s="55"/>
-      <c r="B210" s="55"/>
+      <c r="A210" s="58"/>
+      <c r="B210" s="58"/>
       <c r="C210" s="8" t="s">
         <v>402</v>
       </c>
@@ -29632,8 +29636,8 @@
       </c>
     </row>
     <row r="211" spans="1:8" ht="50" customHeight="1">
-      <c r="A211" s="55"/>
-      <c r="B211" s="55"/>
+      <c r="A211" s="58"/>
+      <c r="B211" s="58"/>
       <c r="C211" s="8" t="s">
         <v>404</v>
       </c>
@@ -29652,8 +29656,8 @@
       </c>
     </row>
     <row r="212" spans="1:8" ht="50" customHeight="1">
-      <c r="A212" s="55"/>
-      <c r="B212" s="55"/>
+      <c r="A212" s="58"/>
+      <c r="B212" s="58"/>
       <c r="C212" s="8" t="s">
         <v>406</v>
       </c>
@@ -29672,8 +29676,8 @@
       </c>
     </row>
     <row r="213" spans="1:8" ht="50" customHeight="1">
-      <c r="A213" s="55"/>
-      <c r="B213" s="55"/>
+      <c r="A213" s="58"/>
+      <c r="B213" s="58"/>
       <c r="C213" s="8" t="s">
         <v>408</v>
       </c>
@@ -29692,8 +29696,8 @@
       </c>
     </row>
     <row r="214" spans="1:8" ht="50" customHeight="1">
-      <c r="A214" s="55"/>
-      <c r="B214" s="55"/>
+      <c r="A214" s="58"/>
+      <c r="B214" s="58"/>
       <c r="C214" s="8" t="s">
         <v>410</v>
       </c>
@@ -29712,8 +29716,8 @@
       </c>
     </row>
     <row r="215" spans="1:8" ht="50" customHeight="1">
-      <c r="A215" s="55"/>
-      <c r="B215" s="55"/>
+      <c r="A215" s="58"/>
+      <c r="B215" s="58"/>
       <c r="C215" s="8" t="s">
         <v>412</v>
       </c>
@@ -29732,8 +29736,8 @@
       </c>
     </row>
     <row r="216" spans="1:8" ht="50" customHeight="1">
-      <c r="A216" s="55"/>
-      <c r="B216" s="55"/>
+      <c r="A216" s="58"/>
+      <c r="B216" s="58"/>
       <c r="C216" s="8" t="s">
         <v>414</v>
       </c>
@@ -29752,8 +29756,8 @@
       </c>
     </row>
     <row r="217" spans="1:8" ht="50" customHeight="1">
-      <c r="A217" s="55"/>
-      <c r="B217" s="55"/>
+      <c r="A217" s="58"/>
+      <c r="B217" s="58"/>
       <c r="C217" s="8" t="s">
         <v>416</v>
       </c>
@@ -29772,8 +29776,8 @@
       </c>
     </row>
     <row r="218" spans="1:8" ht="50" customHeight="1">
-      <c r="A218" s="55"/>
-      <c r="B218" s="55"/>
+      <c r="A218" s="58"/>
+      <c r="B218" s="58"/>
       <c r="C218" s="8" t="s">
         <v>418</v>
       </c>
@@ -29792,8 +29796,8 @@
       </c>
     </row>
     <row r="219" spans="1:8" ht="50" customHeight="1">
-      <c r="A219" s="55"/>
-      <c r="B219" s="55"/>
+      <c r="A219" s="58"/>
+      <c r="B219" s="58"/>
       <c r="C219" s="8" t="s">
         <v>420</v>
       </c>
@@ -29812,8 +29816,8 @@
       </c>
     </row>
     <row r="220" spans="1:8" ht="50" customHeight="1">
-      <c r="A220" s="55"/>
-      <c r="B220" s="55"/>
+      <c r="A220" s="58"/>
+      <c r="B220" s="58"/>
       <c r="C220" s="8" t="s">
         <v>422</v>
       </c>
@@ -29832,8 +29836,8 @@
       </c>
     </row>
     <row r="221" spans="1:8" ht="50" customHeight="1">
-      <c r="A221" s="55"/>
-      <c r="B221" s="55"/>
+      <c r="A221" s="58"/>
+      <c r="B221" s="58"/>
       <c r="C221" s="8" t="s">
         <v>424</v>
       </c>
@@ -29852,8 +29856,8 @@
       </c>
     </row>
     <row r="222" spans="1:8" ht="50" customHeight="1">
-      <c r="A222" s="55"/>
-      <c r="B222" s="55"/>
+      <c r="A222" s="58"/>
+      <c r="B222" s="58"/>
       <c r="C222" s="8" t="s">
         <v>426</v>
       </c>
@@ -29872,8 +29876,8 @@
       </c>
     </row>
     <row r="223" spans="1:8" ht="50" customHeight="1">
-      <c r="A223" s="55"/>
-      <c r="B223" s="56"/>
+      <c r="A223" s="58"/>
+      <c r="B223" s="59"/>
       <c r="C223" s="8" t="s">
         <v>428</v>
       </c>
@@ -29892,8 +29896,8 @@
       </c>
     </row>
     <row r="224" spans="1:8" ht="50" customHeight="1">
-      <c r="A224" s="55"/>
-      <c r="B224" s="54" t="s">
+      <c r="A224" s="58"/>
+      <c r="B224" s="57" t="s">
         <v>877</v>
       </c>
       <c r="C224" s="13" t="s">
@@ -29913,8 +29917,8 @@
       </c>
     </row>
     <row r="225" spans="1:8" ht="50" customHeight="1">
-      <c r="A225" s="55"/>
-      <c r="B225" s="55"/>
+      <c r="A225" s="58"/>
+      <c r="B225" s="58"/>
       <c r="C225" s="13" t="s">
         <v>432</v>
       </c>
@@ -29932,8 +29936,8 @@
       </c>
     </row>
     <row r="226" spans="1:8" ht="50" customHeight="1">
-      <c r="A226" s="55"/>
-      <c r="B226" s="55"/>
+      <c r="A226" s="58"/>
+      <c r="B226" s="58"/>
       <c r="C226" s="13" t="s">
         <v>434</v>
       </c>
@@ -29951,8 +29955,8 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="50" customHeight="1">
-      <c r="A227" s="56"/>
-      <c r="B227" s="56"/>
+      <c r="A227" s="59"/>
+      <c r="B227" s="59"/>
       <c r="C227" s="13" t="s">
         <v>436</v>
       </c>
@@ -29970,7 +29974,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="50" customHeight="1">
-      <c r="A228" s="54" t="s">
+      <c r="A228" s="57" t="s">
         <v>860</v>
       </c>
       <c r="B228" s="14" t="s">
@@ -29994,7 +29998,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="50" customHeight="1">
-      <c r="A229" s="55"/>
+      <c r="A229" s="58"/>
       <c r="B229" s="14" t="s">
         <v>879</v>
       </c>
@@ -30016,8 +30020,8 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="50" customHeight="1">
-      <c r="A230" s="55"/>
-      <c r="B230" s="54" t="s">
+      <c r="A230" s="58"/>
+      <c r="B230" s="57" t="s">
         <v>880</v>
       </c>
       <c r="C230" s="8" t="s">
@@ -30038,8 +30042,8 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="50" customHeight="1">
-      <c r="A231" s="55"/>
-      <c r="B231" s="56"/>
+      <c r="A231" s="58"/>
+      <c r="B231" s="59"/>
       <c r="C231" s="8" t="s">
         <v>444</v>
       </c>
@@ -30058,8 +30062,8 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="50" customHeight="1">
-      <c r="A232" s="55"/>
-      <c r="B232" s="54" t="s">
+      <c r="A232" s="58"/>
+      <c r="B232" s="57" t="s">
         <v>881</v>
       </c>
       <c r="C232" s="8" t="s">
@@ -30080,8 +30084,8 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="50" customHeight="1">
-      <c r="A233" s="55"/>
-      <c r="B233" s="56"/>
+      <c r="A233" s="58"/>
+      <c r="B233" s="59"/>
       <c r="C233" s="8" t="s">
         <v>448</v>
       </c>
@@ -30100,8 +30104,8 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="50" customHeight="1">
-      <c r="A234" s="55"/>
-      <c r="B234" s="54" t="s">
+      <c r="A234" s="58"/>
+      <c r="B234" s="57" t="s">
         <v>882</v>
       </c>
       <c r="C234" s="8" t="s">
@@ -30122,8 +30126,8 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="50" customHeight="1">
-      <c r="A235" s="55"/>
-      <c r="B235" s="55"/>
+      <c r="A235" s="58"/>
+      <c r="B235" s="58"/>
       <c r="C235" s="8" t="s">
         <v>452</v>
       </c>
@@ -30142,8 +30146,8 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="50" customHeight="1">
-      <c r="A236" s="55"/>
-      <c r="B236" s="55"/>
+      <c r="A236" s="58"/>
+      <c r="B236" s="58"/>
       <c r="C236" s="8" t="s">
         <v>454</v>
       </c>
@@ -30162,8 +30166,8 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="50" customHeight="1">
-      <c r="A237" s="55"/>
-      <c r="B237" s="55"/>
+      <c r="A237" s="58"/>
+      <c r="B237" s="58"/>
       <c r="C237" s="8" t="s">
         <v>456</v>
       </c>
@@ -30182,8 +30186,8 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="50" customHeight="1">
-      <c r="A238" s="55"/>
-      <c r="B238" s="55"/>
+      <c r="A238" s="58"/>
+      <c r="B238" s="58"/>
       <c r="C238" s="8" t="s">
         <v>458</v>
       </c>
@@ -30202,8 +30206,8 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="50" customHeight="1">
-      <c r="A239" s="55"/>
-      <c r="B239" s="55"/>
+      <c r="A239" s="58"/>
+      <c r="B239" s="58"/>
       <c r="C239" s="8" t="s">
         <v>460</v>
       </c>
@@ -30222,8 +30226,8 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="50" customHeight="1">
-      <c r="A240" s="55"/>
-      <c r="B240" s="55"/>
+      <c r="A240" s="58"/>
+      <c r="B240" s="58"/>
       <c r="C240" s="8" t="s">
         <v>462</v>
       </c>
@@ -30242,8 +30246,8 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="50" customHeight="1">
-      <c r="A241" s="55"/>
-      <c r="B241" s="55"/>
+      <c r="A241" s="58"/>
+      <c r="B241" s="58"/>
       <c r="C241" s="8" t="s">
         <v>464</v>
       </c>
@@ -30262,8 +30266,8 @@
       </c>
     </row>
     <row r="242" spans="1:8" ht="50" customHeight="1">
-      <c r="A242" s="55"/>
-      <c r="B242" s="55"/>
+      <c r="A242" s="58"/>
+      <c r="B242" s="58"/>
       <c r="C242" s="8" t="s">
         <v>466</v>
       </c>
@@ -30282,8 +30286,8 @@
       </c>
     </row>
     <row r="243" spans="1:8" ht="50" customHeight="1">
-      <c r="A243" s="55"/>
-      <c r="B243" s="55"/>
+      <c r="A243" s="58"/>
+      <c r="B243" s="58"/>
       <c r="C243" s="8" t="s">
         <v>468</v>
       </c>
@@ -30302,8 +30306,8 @@
       </c>
     </row>
     <row r="244" spans="1:8" ht="50" customHeight="1">
-      <c r="A244" s="55"/>
-      <c r="B244" s="55"/>
+      <c r="A244" s="58"/>
+      <c r="B244" s="58"/>
       <c r="C244" s="8" t="s">
         <v>470</v>
       </c>
@@ -30322,8 +30326,8 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="50" customHeight="1">
-      <c r="A245" s="55"/>
-      <c r="B245" s="55"/>
+      <c r="A245" s="58"/>
+      <c r="B245" s="58"/>
       <c r="C245" s="8" t="s">
         <v>472</v>
       </c>
@@ -30342,8 +30346,8 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="50" customHeight="1">
-      <c r="A246" s="55"/>
-      <c r="B246" s="55"/>
+      <c r="A246" s="58"/>
+      <c r="B246" s="58"/>
       <c r="C246" s="8" t="s">
         <v>474</v>
       </c>
@@ -30362,8 +30366,8 @@
       </c>
     </row>
     <row r="247" spans="1:8" ht="50" customHeight="1">
-      <c r="A247" s="55"/>
-      <c r="B247" s="55"/>
+      <c r="A247" s="58"/>
+      <c r="B247" s="58"/>
       <c r="C247" s="8" t="s">
         <v>476</v>
       </c>
@@ -30382,8 +30386,8 @@
       </c>
     </row>
     <row r="248" spans="1:8" ht="50" customHeight="1">
-      <c r="A248" s="55"/>
-      <c r="B248" s="55"/>
+      <c r="A248" s="58"/>
+      <c r="B248" s="58"/>
       <c r="C248" s="8" t="s">
         <v>478</v>
       </c>
@@ -30402,8 +30406,8 @@
       </c>
     </row>
     <row r="249" spans="1:8" ht="50" customHeight="1">
-      <c r="A249" s="55"/>
-      <c r="B249" s="55"/>
+      <c r="A249" s="58"/>
+      <c r="B249" s="58"/>
       <c r="C249" s="8" t="s">
         <v>480</v>
       </c>
@@ -30422,8 +30426,8 @@
       </c>
     </row>
     <row r="250" spans="1:8" ht="50" customHeight="1">
-      <c r="A250" s="55"/>
-      <c r="B250" s="55"/>
+      <c r="A250" s="58"/>
+      <c r="B250" s="58"/>
       <c r="C250" s="8" t="s">
         <v>482</v>
       </c>
@@ -30442,8 +30446,8 @@
       </c>
     </row>
     <row r="251" spans="1:8" ht="50" customHeight="1">
-      <c r="A251" s="55"/>
-      <c r="B251" s="55"/>
+      <c r="A251" s="58"/>
+      <c r="B251" s="58"/>
       <c r="C251" s="8" t="s">
         <v>484</v>
       </c>
@@ -30462,8 +30466,8 @@
       </c>
     </row>
     <row r="252" spans="1:8" ht="50" customHeight="1">
-      <c r="A252" s="55"/>
-      <c r="B252" s="55"/>
+      <c r="A252" s="58"/>
+      <c r="B252" s="58"/>
       <c r="C252" s="8" t="s">
         <v>486</v>
       </c>
@@ -30482,8 +30486,8 @@
       </c>
     </row>
     <row r="253" spans="1:8" ht="50" customHeight="1">
-      <c r="A253" s="55"/>
-      <c r="B253" s="55"/>
+      <c r="A253" s="58"/>
+      <c r="B253" s="58"/>
       <c r="C253" s="8" t="s">
         <v>488</v>
       </c>
@@ -30502,8 +30506,8 @@
       </c>
     </row>
     <row r="254" spans="1:8" ht="50" customHeight="1">
-      <c r="A254" s="55"/>
-      <c r="B254" s="55"/>
+      <c r="A254" s="58"/>
+      <c r="B254" s="58"/>
       <c r="C254" s="8" t="s">
         <v>490</v>
       </c>
@@ -30522,8 +30526,8 @@
       </c>
     </row>
     <row r="255" spans="1:8" ht="50" customHeight="1">
-      <c r="A255" s="55"/>
-      <c r="B255" s="55"/>
+      <c r="A255" s="58"/>
+      <c r="B255" s="58"/>
       <c r="C255" s="8" t="s">
         <v>492</v>
       </c>
@@ -30542,8 +30546,8 @@
       </c>
     </row>
     <row r="256" spans="1:8" ht="50" customHeight="1">
-      <c r="A256" s="55"/>
-      <c r="B256" s="55"/>
+      <c r="A256" s="58"/>
+      <c r="B256" s="58"/>
       <c r="C256" s="8" t="s">
         <v>494</v>
       </c>
@@ -30562,8 +30566,8 @@
       </c>
     </row>
     <row r="257" spans="1:8" ht="50" customHeight="1">
-      <c r="A257" s="55"/>
-      <c r="B257" s="55"/>
+      <c r="A257" s="58"/>
+      <c r="B257" s="58"/>
       <c r="C257" s="8" t="s">
         <v>496</v>
       </c>
@@ -30582,8 +30586,8 @@
       </c>
     </row>
     <row r="258" spans="1:8" ht="50" customHeight="1">
-      <c r="A258" s="55"/>
-      <c r="B258" s="55"/>
+      <c r="A258" s="58"/>
+      <c r="B258" s="58"/>
       <c r="C258" s="8" t="s">
         <v>498</v>
       </c>
@@ -30602,8 +30606,8 @@
       </c>
     </row>
     <row r="259" spans="1:8" ht="50" customHeight="1">
-      <c r="A259" s="55"/>
-      <c r="B259" s="55"/>
+      <c r="A259" s="58"/>
+      <c r="B259" s="58"/>
       <c r="C259" s="8" t="s">
         <v>500</v>
       </c>
@@ -30622,8 +30626,8 @@
       </c>
     </row>
     <row r="260" spans="1:8" ht="50" customHeight="1">
-      <c r="A260" s="55"/>
-      <c r="B260" s="55"/>
+      <c r="A260" s="58"/>
+      <c r="B260" s="58"/>
       <c r="C260" s="8" t="s">
         <v>502</v>
       </c>
@@ -30642,8 +30646,8 @@
       </c>
     </row>
     <row r="261" spans="1:8" ht="50" customHeight="1">
-      <c r="A261" s="55"/>
-      <c r="B261" s="55"/>
+      <c r="A261" s="58"/>
+      <c r="B261" s="58"/>
       <c r="C261" s="8" t="s">
         <v>504</v>
       </c>
@@ -30662,8 +30666,8 @@
       </c>
     </row>
     <row r="262" spans="1:8" ht="50" customHeight="1">
-      <c r="A262" s="55"/>
-      <c r="B262" s="55"/>
+      <c r="A262" s="58"/>
+      <c r="B262" s="58"/>
       <c r="C262" s="8" t="s">
         <v>506</v>
       </c>
@@ -30682,8 +30686,8 @@
       </c>
     </row>
     <row r="263" spans="1:8" ht="50" customHeight="1">
-      <c r="A263" s="55"/>
-      <c r="B263" s="55"/>
+      <c r="A263" s="58"/>
+      <c r="B263" s="58"/>
       <c r="C263" s="8" t="s">
         <v>508</v>
       </c>
@@ -30702,8 +30706,8 @@
       </c>
     </row>
     <row r="264" spans="1:8" ht="50" customHeight="1">
-      <c r="A264" s="55"/>
-      <c r="B264" s="55"/>
+      <c r="A264" s="58"/>
+      <c r="B264" s="58"/>
       <c r="C264" s="8" t="s">
         <v>510</v>
       </c>
@@ -30722,8 +30726,8 @@
       </c>
     </row>
     <row r="265" spans="1:8" ht="50" customHeight="1">
-      <c r="A265" s="55"/>
-      <c r="B265" s="55"/>
+      <c r="A265" s="58"/>
+      <c r="B265" s="58"/>
       <c r="C265" s="8" t="s">
         <v>512</v>
       </c>
@@ -30742,8 +30746,8 @@
       </c>
     </row>
     <row r="266" spans="1:8" ht="50" customHeight="1">
-      <c r="A266" s="55"/>
-      <c r="B266" s="55"/>
+      <c r="A266" s="58"/>
+      <c r="B266" s="58"/>
       <c r="C266" s="8" t="s">
         <v>514</v>
       </c>
@@ -30762,8 +30766,8 @@
       </c>
     </row>
     <row r="267" spans="1:8" ht="50" customHeight="1">
-      <c r="A267" s="55"/>
-      <c r="B267" s="55"/>
+      <c r="A267" s="58"/>
+      <c r="B267" s="58"/>
       <c r="C267" s="8" t="s">
         <v>516</v>
       </c>
@@ -30782,8 +30786,8 @@
       </c>
     </row>
     <row r="268" spans="1:8" ht="50" customHeight="1">
-      <c r="A268" s="55"/>
-      <c r="B268" s="56"/>
+      <c r="A268" s="58"/>
+      <c r="B268" s="59"/>
       <c r="C268" s="8" t="s">
         <v>518</v>
       </c>
@@ -30802,7 +30806,7 @@
       </c>
     </row>
     <row r="269" spans="1:8" ht="50" customHeight="1">
-      <c r="A269" s="55"/>
+      <c r="A269" s="58"/>
       <c r="B269" s="14" t="s">
         <v>883</v>
       </c>
@@ -30824,8 +30828,8 @@
       </c>
     </row>
     <row r="270" spans="1:8" ht="50" customHeight="1">
-      <c r="A270" s="55"/>
-      <c r="B270" s="54" t="s">
+      <c r="A270" s="58"/>
+      <c r="B270" s="57" t="s">
         <v>884</v>
       </c>
       <c r="C270" s="35" t="s">
@@ -30846,8 +30850,8 @@
       </c>
     </row>
     <row r="271" spans="1:8" ht="50" customHeight="1">
-      <c r="A271" s="55"/>
-      <c r="B271" s="55"/>
+      <c r="A271" s="58"/>
+      <c r="B271" s="58"/>
       <c r="C271" s="8" t="s">
         <v>522</v>
       </c>
@@ -30866,8 +30870,8 @@
       </c>
     </row>
     <row r="272" spans="1:8" ht="50" customHeight="1">
-      <c r="A272" s="55"/>
-      <c r="B272" s="55"/>
+      <c r="A272" s="58"/>
+      <c r="B272" s="58"/>
       <c r="C272" s="8" t="s">
         <v>524</v>
       </c>
@@ -30886,8 +30890,8 @@
       </c>
     </row>
     <row r="273" spans="1:8" ht="50" customHeight="1">
-      <c r="A273" s="55"/>
-      <c r="B273" s="55"/>
+      <c r="A273" s="58"/>
+      <c r="B273" s="58"/>
       <c r="C273" s="8" t="s">
         <v>526</v>
       </c>
@@ -30906,8 +30910,8 @@
       </c>
     </row>
     <row r="274" spans="1:8" ht="50" customHeight="1">
-      <c r="A274" s="55"/>
-      <c r="B274" s="56"/>
+      <c r="A274" s="58"/>
+      <c r="B274" s="59"/>
       <c r="C274" s="8" t="s">
         <v>528</v>
       </c>
@@ -30926,8 +30930,8 @@
       </c>
     </row>
     <row r="275" spans="1:8" ht="50" customHeight="1">
-      <c r="A275" s="55"/>
-      <c r="B275" s="54" t="s">
+      <c r="A275" s="58"/>
+      <c r="B275" s="57" t="s">
         <v>885</v>
       </c>
       <c r="C275" s="8" t="s">
@@ -30948,8 +30952,8 @@
       </c>
     </row>
     <row r="276" spans="1:8" ht="50" customHeight="1">
-      <c r="A276" s="55"/>
-      <c r="B276" s="55"/>
+      <c r="A276" s="58"/>
+      <c r="B276" s="58"/>
       <c r="C276" s="8" t="s">
         <v>532</v>
       </c>
@@ -30968,8 +30972,8 @@
       </c>
     </row>
     <row r="277" spans="1:8" ht="50" customHeight="1">
-      <c r="A277" s="55"/>
-      <c r="B277" s="55"/>
+      <c r="A277" s="58"/>
+      <c r="B277" s="58"/>
       <c r="C277" s="8" t="s">
         <v>534</v>
       </c>
@@ -30988,8 +30992,8 @@
       </c>
     </row>
     <row r="278" spans="1:8" ht="50" customHeight="1">
-      <c r="A278" s="55"/>
-      <c r="B278" s="55"/>
+      <c r="A278" s="58"/>
+      <c r="B278" s="58"/>
       <c r="C278" s="8" t="s">
         <v>536</v>
       </c>
@@ -31008,8 +31012,8 @@
       </c>
     </row>
     <row r="279" spans="1:8" ht="50" customHeight="1">
-      <c r="A279" s="55"/>
-      <c r="B279" s="55"/>
+      <c r="A279" s="58"/>
+      <c r="B279" s="58"/>
       <c r="C279" s="8" t="s">
         <v>538</v>
       </c>
@@ -31028,8 +31032,8 @@
       </c>
     </row>
     <row r="280" spans="1:8" ht="50" customHeight="1">
-      <c r="A280" s="55"/>
-      <c r="B280" s="55"/>
+      <c r="A280" s="58"/>
+      <c r="B280" s="58"/>
       <c r="C280" s="8" t="s">
         <v>540</v>
       </c>
@@ -31048,8 +31052,8 @@
       </c>
     </row>
     <row r="281" spans="1:8" ht="50" customHeight="1">
-      <c r="A281" s="55"/>
-      <c r="B281" s="55"/>
+      <c r="A281" s="58"/>
+      <c r="B281" s="58"/>
       <c r="C281" s="8" t="s">
         <v>542</v>
       </c>
@@ -31068,8 +31072,8 @@
       </c>
     </row>
     <row r="282" spans="1:8" ht="50" customHeight="1">
-      <c r="A282" s="55"/>
-      <c r="B282" s="55"/>
+      <c r="A282" s="58"/>
+      <c r="B282" s="58"/>
       <c r="C282" s="8" t="s">
         <v>544</v>
       </c>
@@ -31088,8 +31092,8 @@
       </c>
     </row>
     <row r="283" spans="1:8" ht="50" customHeight="1">
-      <c r="A283" s="55"/>
-      <c r="B283" s="55"/>
+      <c r="A283" s="58"/>
+      <c r="B283" s="58"/>
       <c r="C283" s="8" t="s">
         <v>546</v>
       </c>
@@ -31108,8 +31112,8 @@
       </c>
     </row>
     <row r="284" spans="1:8" ht="50" customHeight="1">
-      <c r="A284" s="55"/>
-      <c r="B284" s="55"/>
+      <c r="A284" s="58"/>
+      <c r="B284" s="58"/>
       <c r="C284" s="8" t="s">
         <v>548</v>
       </c>
@@ -31128,8 +31132,8 @@
       </c>
     </row>
     <row r="285" spans="1:8" ht="50" customHeight="1">
-      <c r="A285" s="55"/>
-      <c r="B285" s="55"/>
+      <c r="A285" s="58"/>
+      <c r="B285" s="58"/>
       <c r="C285" s="8" t="s">
         <v>550</v>
       </c>
@@ -31148,8 +31152,8 @@
       </c>
     </row>
     <row r="286" spans="1:8" ht="50" customHeight="1">
-      <c r="A286" s="55"/>
-      <c r="B286" s="55"/>
+      <c r="A286" s="58"/>
+      <c r="B286" s="58"/>
       <c r="C286" s="8" t="s">
         <v>552</v>
       </c>
@@ -31168,8 +31172,8 @@
       </c>
     </row>
     <row r="287" spans="1:8" ht="50" customHeight="1">
-      <c r="A287" s="55"/>
-      <c r="B287" s="55"/>
+      <c r="A287" s="58"/>
+      <c r="B287" s="58"/>
       <c r="C287" s="8" t="s">
         <v>554</v>
       </c>
@@ -31188,8 +31192,8 @@
       </c>
     </row>
     <row r="288" spans="1:8" ht="50" customHeight="1">
-      <c r="A288" s="55"/>
-      <c r="B288" s="55"/>
+      <c r="A288" s="58"/>
+      <c r="B288" s="58"/>
       <c r="C288" s="8" t="s">
         <v>556</v>
       </c>
@@ -31208,8 +31212,8 @@
       </c>
     </row>
     <row r="289" spans="1:8" ht="50" customHeight="1">
-      <c r="A289" s="55"/>
-      <c r="B289" s="55"/>
+      <c r="A289" s="58"/>
+      <c r="B289" s="58"/>
       <c r="C289" s="8" t="s">
         <v>558</v>
       </c>
@@ -31228,8 +31232,8 @@
       </c>
     </row>
     <row r="290" spans="1:8" ht="50" customHeight="1">
-      <c r="A290" s="55"/>
-      <c r="B290" s="55"/>
+      <c r="A290" s="58"/>
+      <c r="B290" s="58"/>
       <c r="C290" s="8" t="s">
         <v>560</v>
       </c>
@@ -31248,8 +31252,8 @@
       </c>
     </row>
     <row r="291" spans="1:8" ht="50" customHeight="1">
-      <c r="A291" s="55"/>
-      <c r="B291" s="55"/>
+      <c r="A291" s="58"/>
+      <c r="B291" s="58"/>
       <c r="C291" s="8" t="s">
         <v>562</v>
       </c>
@@ -31268,8 +31272,8 @@
       </c>
     </row>
     <row r="292" spans="1:8" ht="50" customHeight="1">
-      <c r="A292" s="55"/>
-      <c r="B292" s="55"/>
+      <c r="A292" s="58"/>
+      <c r="B292" s="58"/>
       <c r="C292" s="8" t="s">
         <v>564</v>
       </c>
@@ -31288,8 +31292,8 @@
       </c>
     </row>
     <row r="293" spans="1:8" ht="50" customHeight="1">
-      <c r="A293" s="55"/>
-      <c r="B293" s="55"/>
+      <c r="A293" s="58"/>
+      <c r="B293" s="58"/>
       <c r="C293" s="8" t="s">
         <v>566</v>
       </c>
@@ -31308,8 +31312,8 @@
       </c>
     </row>
     <row r="294" spans="1:8" ht="50" customHeight="1">
-      <c r="A294" s="55"/>
-      <c r="B294" s="55"/>
+      <c r="A294" s="58"/>
+      <c r="B294" s="58"/>
       <c r="C294" s="8" t="s">
         <v>568</v>
       </c>
@@ -31328,8 +31332,8 @@
       </c>
     </row>
     <row r="295" spans="1:8" ht="50" customHeight="1">
-      <c r="A295" s="55"/>
-      <c r="B295" s="55"/>
+      <c r="A295" s="58"/>
+      <c r="B295" s="58"/>
       <c r="C295" s="8" t="s">
         <v>570</v>
       </c>
@@ -31348,8 +31352,8 @@
       </c>
     </row>
     <row r="296" spans="1:8" ht="50" customHeight="1">
-      <c r="A296" s="55"/>
-      <c r="B296" s="55"/>
+      <c r="A296" s="58"/>
+      <c r="B296" s="58"/>
       <c r="C296" s="8" t="s">
         <v>572</v>
       </c>
@@ -31368,8 +31372,8 @@
       </c>
     </row>
     <row r="297" spans="1:8" ht="50" customHeight="1">
-      <c r="A297" s="55"/>
-      <c r="B297" s="55"/>
+      <c r="A297" s="58"/>
+      <c r="B297" s="58"/>
       <c r="C297" s="8" t="s">
         <v>574</v>
       </c>
@@ -31388,8 +31392,8 @@
       </c>
     </row>
     <row r="298" spans="1:8" ht="50" customHeight="1">
-      <c r="A298" s="55"/>
-      <c r="B298" s="55"/>
+      <c r="A298" s="58"/>
+      <c r="B298" s="58"/>
       <c r="C298" s="8" t="s">
         <v>576</v>
       </c>
@@ -31408,8 +31412,8 @@
       </c>
     </row>
     <row r="299" spans="1:8" ht="50" customHeight="1">
-      <c r="A299" s="55"/>
-      <c r="B299" s="55"/>
+      <c r="A299" s="58"/>
+      <c r="B299" s="58"/>
       <c r="C299" s="8" t="s">
         <v>578</v>
       </c>
@@ -31428,8 +31432,8 @@
       </c>
     </row>
     <row r="300" spans="1:8" ht="50" customHeight="1">
-      <c r="A300" s="55"/>
-      <c r="B300" s="55"/>
+      <c r="A300" s="58"/>
+      <c r="B300" s="58"/>
       <c r="C300" s="8" t="s">
         <v>580</v>
       </c>
@@ -31448,8 +31452,8 @@
       </c>
     </row>
     <row r="301" spans="1:8" ht="50" customHeight="1">
-      <c r="A301" s="55"/>
-      <c r="B301" s="55"/>
+      <c r="A301" s="58"/>
+      <c r="B301" s="58"/>
       <c r="C301" s="8" t="s">
         <v>582</v>
       </c>
@@ -31468,8 +31472,8 @@
       </c>
     </row>
     <row r="302" spans="1:8" ht="50" customHeight="1">
-      <c r="A302" s="55"/>
-      <c r="B302" s="55"/>
+      <c r="A302" s="58"/>
+      <c r="B302" s="58"/>
       <c r="C302" s="8" t="s">
         <v>584</v>
       </c>
@@ -31488,8 +31492,8 @@
       </c>
     </row>
     <row r="303" spans="1:8" ht="50" customHeight="1">
-      <c r="A303" s="55"/>
-      <c r="B303" s="55"/>
+      <c r="A303" s="58"/>
+      <c r="B303" s="58"/>
       <c r="C303" s="8" t="s">
         <v>586</v>
       </c>
@@ -31508,8 +31512,8 @@
       </c>
     </row>
     <row r="304" spans="1:8" ht="50" customHeight="1">
-      <c r="A304" s="55"/>
-      <c r="B304" s="55"/>
+      <c r="A304" s="58"/>
+      <c r="B304" s="58"/>
       <c r="C304" s="8" t="s">
         <v>588</v>
       </c>
@@ -31528,8 +31532,8 @@
       </c>
     </row>
     <row r="305" spans="1:8" ht="50" customHeight="1">
-      <c r="A305" s="55"/>
-      <c r="B305" s="55"/>
+      <c r="A305" s="58"/>
+      <c r="B305" s="58"/>
       <c r="C305" s="8" t="s">
         <v>590</v>
       </c>
@@ -31548,8 +31552,8 @@
       </c>
     </row>
     <row r="306" spans="1:8" ht="50" customHeight="1">
-      <c r="A306" s="55"/>
-      <c r="B306" s="55"/>
+      <c r="A306" s="58"/>
+      <c r="B306" s="58"/>
       <c r="C306" s="8" t="s">
         <v>592</v>
       </c>
@@ -31568,8 +31572,8 @@
       </c>
     </row>
     <row r="307" spans="1:8" ht="50" customHeight="1">
-      <c r="A307" s="55"/>
-      <c r="B307" s="56"/>
+      <c r="A307" s="58"/>
+      <c r="B307" s="59"/>
       <c r="C307" s="8" t="s">
         <v>594</v>
       </c>
@@ -31588,7 +31592,7 @@
       </c>
     </row>
     <row r="308" spans="1:8" ht="50" customHeight="1">
-      <c r="A308" s="55"/>
+      <c r="A308" s="58"/>
       <c r="B308" s="14" t="s">
         <v>886</v>
       </c>
@@ -31610,7 +31614,7 @@
       </c>
     </row>
     <row r="309" spans="1:8" ht="50" customHeight="1">
-      <c r="A309" s="55"/>
+      <c r="A309" s="58"/>
       <c r="B309" s="14" t="s">
         <v>887</v>
       </c>
@@ -31632,8 +31636,8 @@
       </c>
     </row>
     <row r="310" spans="1:8" ht="50" customHeight="1">
-      <c r="A310" s="55"/>
-      <c r="B310" s="54" t="s">
+      <c r="A310" s="58"/>
+      <c r="B310" s="57" t="s">
         <v>888</v>
       </c>
       <c r="C310" s="8" t="s">
@@ -31654,8 +31658,8 @@
       </c>
     </row>
     <row r="311" spans="1:8" ht="50" customHeight="1">
-      <c r="A311" s="55"/>
-      <c r="B311" s="55"/>
+      <c r="A311" s="58"/>
+      <c r="B311" s="58"/>
       <c r="C311" s="8" t="s">
         <v>602</v>
       </c>
@@ -31674,8 +31678,8 @@
       </c>
     </row>
     <row r="312" spans="1:8" ht="50" customHeight="1">
-      <c r="A312" s="55"/>
-      <c r="B312" s="55"/>
+      <c r="A312" s="58"/>
+      <c r="B312" s="58"/>
       <c r="C312" s="8" t="s">
         <v>604</v>
       </c>
@@ -31694,8 +31698,8 @@
       </c>
     </row>
     <row r="313" spans="1:8" ht="50" customHeight="1">
-      <c r="A313" s="55"/>
-      <c r="B313" s="55"/>
+      <c r="A313" s="58"/>
+      <c r="B313" s="58"/>
       <c r="C313" s="35" t="s">
         <v>893</v>
       </c>
@@ -31714,8 +31718,8 @@
       </c>
     </row>
     <row r="314" spans="1:8" ht="50" customHeight="1">
-      <c r="A314" s="55"/>
-      <c r="B314" s="56"/>
+      <c r="A314" s="58"/>
+      <c r="B314" s="59"/>
       <c r="C314" s="35" t="s">
         <v>895</v>
       </c>
@@ -31734,8 +31738,8 @@
       </c>
     </row>
     <row r="315" spans="1:8" ht="50" customHeight="1">
-      <c r="A315" s="55"/>
-      <c r="B315" s="54" t="s">
+      <c r="A315" s="58"/>
+      <c r="B315" s="57" t="s">
         <v>889</v>
       </c>
       <c r="C315" s="8" t="s">
@@ -31756,8 +31760,8 @@
       </c>
     </row>
     <row r="316" spans="1:8" ht="50" customHeight="1">
-      <c r="A316" s="55"/>
-      <c r="B316" s="55"/>
+      <c r="A316" s="58"/>
+      <c r="B316" s="58"/>
       <c r="C316" s="8" t="s">
         <v>608</v>
       </c>
@@ -31776,8 +31780,8 @@
       </c>
     </row>
     <row r="317" spans="1:8" ht="50" customHeight="1">
-      <c r="A317" s="55"/>
-      <c r="B317" s="56"/>
+      <c r="A317" s="58"/>
+      <c r="B317" s="59"/>
       <c r="C317" s="8" t="s">
         <v>610</v>
       </c>
@@ -31796,8 +31800,8 @@
       </c>
     </row>
     <row r="318" spans="1:8" ht="50" customHeight="1">
-      <c r="A318" s="55"/>
-      <c r="B318" s="54" t="s">
+      <c r="A318" s="58"/>
+      <c r="B318" s="57" t="s">
         <v>890</v>
       </c>
       <c r="C318" s="8" t="s">
@@ -31818,8 +31822,8 @@
       </c>
     </row>
     <row r="319" spans="1:8" ht="50" customHeight="1">
-      <c r="A319" s="55"/>
-      <c r="B319" s="55"/>
+      <c r="A319" s="58"/>
+      <c r="B319" s="58"/>
       <c r="C319" s="8" t="s">
         <v>614</v>
       </c>
@@ -31838,8 +31842,8 @@
       </c>
     </row>
     <row r="320" spans="1:8" ht="50" customHeight="1">
-      <c r="A320" s="55"/>
-      <c r="B320" s="55"/>
+      <c r="A320" s="58"/>
+      <c r="B320" s="58"/>
       <c r="C320" s="8" t="s">
         <v>616</v>
       </c>
@@ -31858,8 +31862,8 @@
       </c>
     </row>
     <row r="321" spans="1:8" ht="50" customHeight="1">
-      <c r="A321" s="55"/>
-      <c r="B321" s="55"/>
+      <c r="A321" s="58"/>
+      <c r="B321" s="58"/>
       <c r="C321" s="8" t="s">
         <v>618</v>
       </c>
@@ -31878,8 +31882,8 @@
       </c>
     </row>
     <row r="322" spans="1:8" ht="50" customHeight="1">
-      <c r="A322" s="55"/>
-      <c r="B322" s="55"/>
+      <c r="A322" s="58"/>
+      <c r="B322" s="58"/>
       <c r="C322" s="8" t="s">
         <v>620</v>
       </c>
@@ -31898,8 +31902,8 @@
       </c>
     </row>
     <row r="323" spans="1:8" ht="50" customHeight="1">
-      <c r="A323" s="55"/>
-      <c r="B323" s="55"/>
+      <c r="A323" s="58"/>
+      <c r="B323" s="58"/>
       <c r="C323" s="8" t="s">
         <v>622</v>
       </c>
@@ -31918,8 +31922,8 @@
       </c>
     </row>
     <row r="324" spans="1:8" ht="50" customHeight="1">
-      <c r="A324" s="55"/>
-      <c r="B324" s="55"/>
+      <c r="A324" s="58"/>
+      <c r="B324" s="58"/>
       <c r="C324" s="8" t="s">
         <v>624</v>
       </c>
@@ -31938,8 +31942,8 @@
       </c>
     </row>
     <row r="325" spans="1:8" ht="50" customHeight="1">
-      <c r="A325" s="55"/>
-      <c r="B325" s="55"/>
+      <c r="A325" s="58"/>
+      <c r="B325" s="58"/>
       <c r="C325" s="8" t="s">
         <v>626</v>
       </c>
@@ -31958,8 +31962,8 @@
       </c>
     </row>
     <row r="326" spans="1:8" ht="50" customHeight="1">
-      <c r="A326" s="55"/>
-      <c r="B326" s="55"/>
+      <c r="A326" s="58"/>
+      <c r="B326" s="58"/>
       <c r="C326" s="8" t="s">
         <v>628</v>
       </c>
@@ -31978,8 +31982,8 @@
       </c>
     </row>
     <row r="327" spans="1:8" ht="50" customHeight="1">
-      <c r="A327" s="55"/>
-      <c r="B327" s="56"/>
+      <c r="A327" s="58"/>
+      <c r="B327" s="59"/>
       <c r="C327" s="8" t="s">
         <v>630</v>
       </c>
@@ -31998,7 +32002,7 @@
       </c>
     </row>
     <row r="328" spans="1:8" ht="50" customHeight="1">
-      <c r="A328" s="55"/>
+      <c r="A328" s="58"/>
       <c r="B328" s="14" t="s">
         <v>891</v>
       </c>
@@ -32020,8 +32024,8 @@
       </c>
     </row>
     <row r="329" spans="1:8" ht="50" customHeight="1">
-      <c r="A329" s="55"/>
-      <c r="B329" s="54" t="s">
+      <c r="A329" s="58"/>
+      <c r="B329" s="57" t="s">
         <v>892</v>
       </c>
       <c r="C329" s="8" t="s">
@@ -32042,8 +32046,8 @@
       </c>
     </row>
     <row r="330" spans="1:8" ht="50" customHeight="1">
-      <c r="A330" s="55"/>
-      <c r="B330" s="55"/>
+      <c r="A330" s="58"/>
+      <c r="B330" s="58"/>
       <c r="C330" s="8" t="s">
         <v>636</v>
       </c>
@@ -32062,8 +32066,8 @@
       </c>
     </row>
     <row r="331" spans="1:8" ht="50" customHeight="1">
-      <c r="A331" s="55"/>
-      <c r="B331" s="55"/>
+      <c r="A331" s="58"/>
+      <c r="B331" s="58"/>
       <c r="C331" s="8" t="s">
         <v>638</v>
       </c>
@@ -32080,8 +32084,8 @@
       </c>
     </row>
     <row r="332" spans="1:8" ht="50" customHeight="1">
-      <c r="A332" s="55"/>
-      <c r="B332" s="55"/>
+      <c r="A332" s="58"/>
+      <c r="B332" s="58"/>
       <c r="C332" s="8" t="s">
         <v>640</v>
       </c>
@@ -32100,8 +32104,8 @@
       </c>
     </row>
     <row r="333" spans="1:8" ht="50" customHeight="1">
-      <c r="A333" s="56"/>
-      <c r="B333" s="56"/>
+      <c r="A333" s="59"/>
+      <c r="B333" s="59"/>
       <c r="C333" s="8" t="s">
         <v>642</v>
       </c>
@@ -32120,7 +32124,7 @@
       </c>
     </row>
     <row r="334" spans="1:8" ht="50" customHeight="1">
-      <c r="A334" s="54" t="s">
+      <c r="A334" s="57" t="s">
         <v>861</v>
       </c>
       <c r="C334" s="8" t="s">
@@ -32141,7 +32145,7 @@
       </c>
     </row>
     <row r="335" spans="1:8" ht="50" customHeight="1">
-      <c r="A335" s="55"/>
+      <c r="A335" s="58"/>
       <c r="C335" s="8" t="s">
         <v>646</v>
       </c>
@@ -32160,7 +32164,7 @@
       </c>
     </row>
     <row r="336" spans="1:8" ht="50" customHeight="1">
-      <c r="A336" s="55"/>
+      <c r="A336" s="58"/>
       <c r="C336" s="8" t="s">
         <v>648</v>
       </c>
@@ -32179,7 +32183,7 @@
       </c>
     </row>
     <row r="337" spans="1:8" ht="50" customHeight="1">
-      <c r="A337" s="55"/>
+      <c r="A337" s="58"/>
       <c r="C337" s="8" t="s">
         <v>650</v>
       </c>
@@ -32198,7 +32202,7 @@
       </c>
     </row>
     <row r="338" spans="1:8" ht="50" customHeight="1">
-      <c r="A338" s="55"/>
+      <c r="A338" s="58"/>
       <c r="C338" s="8" t="s">
         <v>652</v>
       </c>
@@ -32217,7 +32221,7 @@
       </c>
     </row>
     <row r="339" spans="1:8" ht="50" customHeight="1">
-      <c r="A339" s="55"/>
+      <c r="A339" s="58"/>
       <c r="C339" s="8" t="s">
         <v>654</v>
       </c>
@@ -32236,7 +32240,7 @@
       </c>
     </row>
     <row r="340" spans="1:8" ht="50" customHeight="1">
-      <c r="A340" s="55"/>
+      <c r="A340" s="58"/>
       <c r="C340" s="8" t="s">
         <v>656</v>
       </c>
@@ -32255,7 +32259,7 @@
       </c>
     </row>
     <row r="341" spans="1:8" ht="50" customHeight="1">
-      <c r="A341" s="55"/>
+      <c r="A341" s="58"/>
       <c r="C341" s="8" t="s">
         <v>658</v>
       </c>
@@ -32274,7 +32278,7 @@
       </c>
     </row>
     <row r="342" spans="1:8" ht="50" customHeight="1">
-      <c r="A342" s="55"/>
+      <c r="A342" s="58"/>
       <c r="C342" s="8" t="s">
         <v>660</v>
       </c>
@@ -32293,7 +32297,7 @@
       </c>
     </row>
     <row r="343" spans="1:8" ht="50" customHeight="1">
-      <c r="A343" s="55"/>
+      <c r="A343" s="58"/>
       <c r="C343" s="8" t="s">
         <v>662</v>
       </c>
@@ -32312,7 +32316,7 @@
       </c>
     </row>
     <row r="344" spans="1:8" ht="50" customHeight="1">
-      <c r="A344" s="55"/>
+      <c r="A344" s="58"/>
       <c r="C344" s="8" t="s">
         <v>664</v>
       </c>
@@ -32331,7 +32335,7 @@
       </c>
     </row>
     <row r="345" spans="1:8" ht="50" customHeight="1">
-      <c r="A345" s="55"/>
+      <c r="A345" s="58"/>
       <c r="C345" s="8" t="s">
         <v>666</v>
       </c>
@@ -32350,7 +32354,7 @@
       </c>
     </row>
     <row r="346" spans="1:8" ht="50" customHeight="1">
-      <c r="A346" s="55"/>
+      <c r="A346" s="58"/>
       <c r="C346" s="8" t="s">
         <v>668</v>
       </c>
@@ -32369,7 +32373,7 @@
       </c>
     </row>
     <row r="347" spans="1:8" ht="50" customHeight="1">
-      <c r="A347" s="55"/>
+      <c r="A347" s="58"/>
       <c r="C347" s="35" t="s">
         <v>910</v>
       </c>
@@ -32388,7 +32392,7 @@
       </c>
     </row>
     <row r="348" spans="1:8" ht="50" customHeight="1">
-      <c r="A348" s="55"/>
+      <c r="A348" s="58"/>
       <c r="C348" s="8" t="s">
         <v>670</v>
       </c>
@@ -32407,7 +32411,7 @@
       </c>
     </row>
     <row r="349" spans="1:8" ht="50" customHeight="1">
-      <c r="A349" s="55"/>
+      <c r="A349" s="58"/>
       <c r="C349" s="8" t="s">
         <v>672</v>
       </c>
@@ -32426,7 +32430,7 @@
       </c>
     </row>
     <row r="350" spans="1:8" ht="50" customHeight="1">
-      <c r="A350" s="55"/>
+      <c r="A350" s="58"/>
       <c r="C350" s="8" t="s">
         <v>674</v>
       </c>
@@ -32445,7 +32449,7 @@
       </c>
     </row>
     <row r="351" spans="1:8" ht="50" customHeight="1">
-      <c r="A351" s="55"/>
+      <c r="A351" s="58"/>
       <c r="C351" s="8" t="s">
         <v>676</v>
       </c>
@@ -32464,7 +32468,7 @@
       </c>
     </row>
     <row r="352" spans="1:8" ht="50" customHeight="1">
-      <c r="A352" s="55"/>
+      <c r="A352" s="58"/>
       <c r="C352" s="8" t="s">
         <v>678</v>
       </c>
@@ -32483,7 +32487,7 @@
       </c>
     </row>
     <row r="353" spans="1:8" ht="50" customHeight="1">
-      <c r="A353" s="55"/>
+      <c r="A353" s="58"/>
       <c r="C353" s="8" t="s">
         <v>680</v>
       </c>
@@ -32502,7 +32506,7 @@
       </c>
     </row>
     <row r="354" spans="1:8" ht="50" customHeight="1">
-      <c r="A354" s="55"/>
+      <c r="A354" s="58"/>
       <c r="C354" s="8" t="s">
         <v>682</v>
       </c>
@@ -32521,7 +32525,7 @@
       </c>
     </row>
     <row r="355" spans="1:8" ht="50" customHeight="1">
-      <c r="A355" s="55"/>
+      <c r="A355" s="58"/>
       <c r="C355" s="8" t="s">
         <v>684</v>
       </c>
@@ -32540,7 +32544,7 @@
       </c>
     </row>
     <row r="356" spans="1:8" ht="50" customHeight="1">
-      <c r="A356" s="55"/>
+      <c r="A356" s="58"/>
       <c r="C356" s="8" t="s">
         <v>686</v>
       </c>
@@ -32559,7 +32563,7 @@
       </c>
     </row>
     <row r="357" spans="1:8" ht="50" customHeight="1">
-      <c r="A357" s="55"/>
+      <c r="A357" s="58"/>
       <c r="C357" s="8" t="s">
         <v>688</v>
       </c>
@@ -32578,7 +32582,7 @@
       </c>
     </row>
     <row r="358" spans="1:8" ht="50" customHeight="1">
-      <c r="A358" s="55"/>
+      <c r="A358" s="58"/>
       <c r="C358" s="8" t="s">
         <v>690</v>
       </c>
@@ -32597,7 +32601,7 @@
       </c>
     </row>
     <row r="359" spans="1:8" ht="50" customHeight="1">
-      <c r="A359" s="55"/>
+      <c r="A359" s="58"/>
       <c r="C359" s="8" t="s">
         <v>692</v>
       </c>
@@ -32616,7 +32620,7 @@
       </c>
     </row>
     <row r="360" spans="1:8" ht="50" customHeight="1">
-      <c r="A360" s="55"/>
+      <c r="A360" s="58"/>
       <c r="C360" s="8" t="s">
         <v>694</v>
       </c>
@@ -32635,7 +32639,7 @@
       </c>
     </row>
     <row r="361" spans="1:8" ht="50" customHeight="1">
-      <c r="A361" s="55"/>
+      <c r="A361" s="58"/>
       <c r="C361" s="8" t="s">
         <v>696</v>
       </c>
@@ -32654,7 +32658,7 @@
       </c>
     </row>
     <row r="362" spans="1:8" ht="50" customHeight="1">
-      <c r="A362" s="55"/>
+      <c r="A362" s="58"/>
       <c r="C362" s="8" t="s">
         <v>698</v>
       </c>
@@ -32673,7 +32677,7 @@
       </c>
     </row>
     <row r="363" spans="1:8" ht="50" customHeight="1">
-      <c r="A363" s="55"/>
+      <c r="A363" s="58"/>
       <c r="C363" s="8" t="s">
         <v>700</v>
       </c>
@@ -32692,7 +32696,7 @@
       </c>
     </row>
     <row r="364" spans="1:8" ht="50" customHeight="1">
-      <c r="A364" s="55"/>
+      <c r="A364" s="58"/>
       <c r="C364" s="8" t="s">
         <v>702</v>
       </c>
@@ -32711,7 +32715,7 @@
       </c>
     </row>
     <row r="365" spans="1:8" ht="50" customHeight="1">
-      <c r="A365" s="55"/>
+      <c r="A365" s="58"/>
       <c r="C365" s="8" t="s">
         <v>704</v>
       </c>
@@ -32730,7 +32734,7 @@
       </c>
     </row>
     <row r="366" spans="1:8" ht="50" customHeight="1">
-      <c r="A366" s="55"/>
+      <c r="A366" s="58"/>
       <c r="C366" s="8" t="s">
         <v>706</v>
       </c>
@@ -32749,7 +32753,7 @@
       </c>
     </row>
     <row r="367" spans="1:8" ht="50" customHeight="1">
-      <c r="A367" s="55"/>
+      <c r="A367" s="58"/>
       <c r="C367" s="8" t="s">
         <v>708</v>
       </c>
@@ -32768,7 +32772,7 @@
       </c>
     </row>
     <row r="368" spans="1:8" ht="50" customHeight="1">
-      <c r="A368" s="55"/>
+      <c r="A368" s="58"/>
       <c r="C368" s="8" t="s">
         <v>710</v>
       </c>
@@ -32787,7 +32791,7 @@
       </c>
     </row>
     <row r="369" spans="1:8" ht="50" customHeight="1">
-      <c r="A369" s="55"/>
+      <c r="A369" s="58"/>
       <c r="C369" s="8" t="s">
         <v>712</v>
       </c>
@@ -32806,7 +32810,7 @@
       </c>
     </row>
     <row r="370" spans="1:8" ht="50" customHeight="1">
-      <c r="A370" s="55"/>
+      <c r="A370" s="58"/>
       <c r="C370" s="8" t="s">
         <v>714</v>
       </c>
@@ -32825,7 +32829,7 @@
       </c>
     </row>
     <row r="371" spans="1:8" ht="50" customHeight="1">
-      <c r="A371" s="55"/>
+      <c r="A371" s="58"/>
       <c r="C371" s="8" t="s">
         <v>716</v>
       </c>
@@ -32844,7 +32848,7 @@
       </c>
     </row>
     <row r="372" spans="1:8" ht="50" customHeight="1">
-      <c r="A372" s="55"/>
+      <c r="A372" s="58"/>
       <c r="C372" s="8" t="s">
         <v>718</v>
       </c>
@@ -32863,7 +32867,7 @@
       </c>
     </row>
     <row r="373" spans="1:8" ht="50" customHeight="1">
-      <c r="A373" s="55"/>
+      <c r="A373" s="58"/>
       <c r="C373" s="8" t="s">
         <v>1014</v>
       </c>
@@ -32874,11 +32878,15 @@
         <v>920</v>
       </c>
       <c r="F373" s="10"/>
-      <c r="G373" s="20"/>
-      <c r="H373" s="45"/>
+      <c r="G373" s="20" t="s">
+        <v>998</v>
+      </c>
+      <c r="H373" s="45" t="s">
+        <v>999</v>
+      </c>
     </row>
     <row r="374" spans="1:8" ht="50" customHeight="1">
-      <c r="A374" s="55"/>
+      <c r="A374" s="58"/>
       <c r="C374" s="8" t="s">
         <v>720</v>
       </c>
@@ -32897,7 +32905,7 @@
       </c>
     </row>
     <row r="375" spans="1:8" ht="50" customHeight="1">
-      <c r="A375" s="55"/>
+      <c r="A375" s="58"/>
       <c r="C375" s="8" t="s">
         <v>722</v>
       </c>
@@ -32916,7 +32924,7 @@
       </c>
     </row>
     <row r="376" spans="1:8" ht="50" customHeight="1">
-      <c r="A376" s="55"/>
+      <c r="A376" s="58"/>
       <c r="C376" s="8" t="s">
         <v>724</v>
       </c>
@@ -32935,7 +32943,7 @@
       </c>
     </row>
     <row r="377" spans="1:8" ht="50" customHeight="1">
-      <c r="A377" s="55"/>
+      <c r="A377" s="58"/>
       <c r="C377" s="8" t="s">
         <v>726</v>
       </c>
@@ -32954,7 +32962,7 @@
       </c>
     </row>
     <row r="378" spans="1:8" ht="50" customHeight="1">
-      <c r="A378" s="55"/>
+      <c r="A378" s="58"/>
       <c r="C378" s="8" t="s">
         <v>728</v>
       </c>
@@ -32973,7 +32981,7 @@
       </c>
     </row>
     <row r="379" spans="1:8" ht="50" customHeight="1">
-      <c r="A379" s="55"/>
+      <c r="A379" s="58"/>
       <c r="C379" s="8" t="s">
         <v>730</v>
       </c>
@@ -32992,7 +33000,7 @@
       </c>
     </row>
     <row r="380" spans="1:8" ht="50" customHeight="1">
-      <c r="A380" s="55"/>
+      <c r="A380" s="58"/>
       <c r="C380" s="8" t="s">
         <v>732</v>
       </c>
@@ -33011,7 +33019,7 @@
       </c>
     </row>
     <row r="381" spans="1:8" ht="50" customHeight="1">
-      <c r="A381" s="55"/>
+      <c r="A381" s="58"/>
       <c r="C381" s="8" t="s">
         <v>734</v>
       </c>
@@ -33030,7 +33038,7 @@
       </c>
     </row>
     <row r="382" spans="1:8" ht="50" customHeight="1">
-      <c r="A382" s="55"/>
+      <c r="A382" s="58"/>
       <c r="C382" s="8" t="s">
         <v>736</v>
       </c>
@@ -33049,7 +33057,7 @@
       </c>
     </row>
     <row r="383" spans="1:8" ht="50" customHeight="1">
-      <c r="A383" s="55"/>
+      <c r="A383" s="58"/>
       <c r="C383" s="8" t="s">
         <v>738</v>
       </c>
@@ -33068,7 +33076,7 @@
       </c>
     </row>
     <row r="384" spans="1:8" ht="50" customHeight="1">
-      <c r="A384" s="55"/>
+      <c r="A384" s="58"/>
       <c r="C384" s="8" t="s">
         <v>740</v>
       </c>
@@ -33087,7 +33095,7 @@
       </c>
     </row>
     <row r="385" spans="1:8" ht="50" customHeight="1">
-      <c r="A385" s="55"/>
+      <c r="A385" s="58"/>
       <c r="C385" s="8" t="s">
         <v>742</v>
       </c>
@@ -33106,7 +33114,7 @@
       </c>
     </row>
     <row r="386" spans="1:8" ht="50" customHeight="1">
-      <c r="A386" s="55"/>
+      <c r="A386" s="58"/>
       <c r="C386" s="8" t="s">
         <v>744</v>
       </c>
@@ -33125,7 +33133,7 @@
       </c>
     </row>
     <row r="387" spans="1:8" ht="50" customHeight="1">
-      <c r="A387" s="55"/>
+      <c r="A387" s="58"/>
       <c r="C387" s="8" t="s">
         <v>746</v>
       </c>
@@ -33144,7 +33152,7 @@
       </c>
     </row>
     <row r="388" spans="1:8" ht="50" customHeight="1">
-      <c r="A388" s="55"/>
+      <c r="A388" s="58"/>
       <c r="C388" s="8" t="s">
         <v>748</v>
       </c>
@@ -33163,7 +33171,7 @@
       </c>
     </row>
     <row r="389" spans="1:8" ht="50" customHeight="1">
-      <c r="A389" s="55"/>
+      <c r="A389" s="58"/>
       <c r="C389" s="8" t="s">
         <v>750</v>
       </c>
@@ -33174,15 +33182,15 @@
         <v>980</v>
       </c>
       <c r="F389" s="10"/>
-      <c r="G389" s="31" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H389" s="51" t="s">
-        <v>1011</v>
+      <c r="G389" s="23" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H389" s="47" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="390" spans="1:8" ht="50" customHeight="1">
-      <c r="A390" s="55"/>
+      <c r="A390" s="58"/>
       <c r="C390" s="8" t="s">
         <v>752</v>
       </c>
@@ -33193,15 +33201,15 @@
         <v>980</v>
       </c>
       <c r="F390" s="10"/>
-      <c r="G390" s="31" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H390" s="51" t="s">
-        <v>1011</v>
+      <c r="G390" s="23" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H390" s="47" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="391" spans="1:8" ht="50" customHeight="1">
-      <c r="A391" s="55"/>
+      <c r="A391" s="58"/>
       <c r="C391" s="8" t="s">
         <v>754</v>
       </c>
@@ -33220,7 +33228,7 @@
       </c>
     </row>
     <row r="392" spans="1:8" ht="50" customHeight="1">
-      <c r="A392" s="55"/>
+      <c r="A392" s="58"/>
       <c r="C392" s="8" t="s">
         <v>756</v>
       </c>
@@ -33239,7 +33247,7 @@
       </c>
     </row>
     <row r="393" spans="1:8" ht="50" customHeight="1">
-      <c r="A393" s="55"/>
+      <c r="A393" s="58"/>
       <c r="C393" s="8" t="s">
         <v>758</v>
       </c>
@@ -33258,7 +33266,7 @@
       </c>
     </row>
     <row r="394" spans="1:8" ht="50" customHeight="1">
-      <c r="A394" s="55"/>
+      <c r="A394" s="58"/>
       <c r="C394" s="8" t="s">
         <v>760</v>
       </c>
@@ -33277,7 +33285,7 @@
       </c>
     </row>
     <row r="395" spans="1:8" ht="50" customHeight="1">
-      <c r="A395" s="55"/>
+      <c r="A395" s="58"/>
       <c r="C395" s="8" t="s">
         <v>762</v>
       </c>
@@ -33296,7 +33304,7 @@
       </c>
     </row>
     <row r="396" spans="1:8" ht="50" customHeight="1">
-      <c r="A396" s="55"/>
+      <c r="A396" s="58"/>
       <c r="C396" s="8" t="s">
         <v>764</v>
       </c>
@@ -33315,7 +33323,7 @@
       </c>
     </row>
     <row r="397" spans="1:8" ht="50" customHeight="1">
-      <c r="A397" s="55"/>
+      <c r="A397" s="58"/>
       <c r="C397" s="8" t="s">
         <v>766</v>
       </c>
@@ -33334,7 +33342,7 @@
       </c>
     </row>
     <row r="398" spans="1:8" ht="50" customHeight="1">
-      <c r="A398" s="55"/>
+      <c r="A398" s="58"/>
       <c r="C398" s="8" t="s">
         <v>768</v>
       </c>
@@ -33353,7 +33361,7 @@
       </c>
     </row>
     <row r="399" spans="1:8" ht="50" customHeight="1">
-      <c r="A399" s="55"/>
+      <c r="A399" s="58"/>
       <c r="C399" s="8" t="s">
         <v>770</v>
       </c>
@@ -33372,7 +33380,7 @@
       </c>
     </row>
     <row r="400" spans="1:8" ht="50" customHeight="1">
-      <c r="A400" s="55"/>
+      <c r="A400" s="58"/>
       <c r="C400" s="8" t="s">
         <v>772</v>
       </c>
@@ -33391,7 +33399,7 @@
       </c>
     </row>
     <row r="401" spans="1:8" ht="50" customHeight="1">
-      <c r="A401" s="55"/>
+      <c r="A401" s="58"/>
       <c r="C401" s="8" t="s">
         <v>774</v>
       </c>
@@ -33410,7 +33418,7 @@
       </c>
     </row>
     <row r="402" spans="1:8" ht="50" customHeight="1">
-      <c r="A402" s="55"/>
+      <c r="A402" s="58"/>
       <c r="C402" s="8" t="s">
         <v>776</v>
       </c>
@@ -33429,7 +33437,7 @@
       </c>
     </row>
     <row r="403" spans="1:8" ht="50" customHeight="1">
-      <c r="A403" s="55"/>
+      <c r="A403" s="58"/>
       <c r="C403" s="8" t="s">
         <v>778</v>
       </c>
@@ -33448,7 +33456,7 @@
       </c>
     </row>
     <row r="404" spans="1:8" ht="50" customHeight="1">
-      <c r="A404" s="55"/>
+      <c r="A404" s="58"/>
       <c r="C404" s="8" t="s">
         <v>780</v>
       </c>
@@ -33467,7 +33475,7 @@
       </c>
     </row>
     <row r="405" spans="1:8" ht="50" customHeight="1">
-      <c r="A405" s="55"/>
+      <c r="A405" s="58"/>
       <c r="C405" s="8" t="s">
         <v>782</v>
       </c>
@@ -33486,7 +33494,7 @@
       </c>
     </row>
     <row r="406" spans="1:8" ht="50" customHeight="1">
-      <c r="A406" s="56"/>
+      <c r="A406" s="59"/>
       <c r="C406" s="8" t="s">
         <v>784</v>
       </c>
@@ -33505,10 +33513,10 @@
       </c>
     </row>
     <row r="407" spans="1:8" ht="50" customHeight="1">
-      <c r="A407" s="54" t="s">
+      <c r="A407" s="57" t="s">
         <v>862</v>
       </c>
-      <c r="B407" s="54" t="s">
+      <c r="B407" s="57" t="s">
         <v>863</v>
       </c>
       <c r="C407" s="26" t="s">
@@ -33528,8 +33536,8 @@
       </c>
     </row>
     <row r="408" spans="1:8" ht="50" customHeight="1">
-      <c r="A408" s="55"/>
-      <c r="B408" s="55"/>
+      <c r="A408" s="58"/>
+      <c r="B408" s="58"/>
       <c r="C408" s="27" t="s">
         <v>788</v>
       </c>
@@ -33548,8 +33556,8 @@
       </c>
     </row>
     <row r="409" spans="1:8" ht="50" customHeight="1">
-      <c r="A409" s="55"/>
-      <c r="B409" s="55"/>
+      <c r="A409" s="58"/>
+      <c r="B409" s="58"/>
       <c r="C409" s="27" t="s">
         <v>790</v>
       </c>
@@ -33568,8 +33576,8 @@
       </c>
     </row>
     <row r="410" spans="1:8" ht="50" customHeight="1">
-      <c r="A410" s="55"/>
-      <c r="B410" s="56"/>
+      <c r="A410" s="58"/>
+      <c r="B410" s="59"/>
       <c r="C410" s="27" t="s">
         <v>792</v>
       </c>
@@ -33588,8 +33596,8 @@
       </c>
     </row>
     <row r="411" spans="1:8" ht="50" customHeight="1">
-      <c r="A411" s="55"/>
-      <c r="B411" s="54" t="s">
+      <c r="A411" s="58"/>
+      <c r="B411" s="57" t="s">
         <v>864</v>
       </c>
       <c r="C411" s="27" t="s">
@@ -33610,8 +33618,8 @@
       </c>
     </row>
     <row r="412" spans="1:8" ht="50" customHeight="1">
-      <c r="A412" s="55"/>
-      <c r="B412" s="55"/>
+      <c r="A412" s="58"/>
+      <c r="B412" s="58"/>
       <c r="C412" s="27" t="s">
         <v>796</v>
       </c>
@@ -33630,8 +33638,8 @@
       </c>
     </row>
     <row r="413" spans="1:8" ht="50" customHeight="1">
-      <c r="A413" s="55"/>
-      <c r="B413" s="55"/>
+      <c r="A413" s="58"/>
+      <c r="B413" s="58"/>
       <c r="C413" s="27" t="s">
         <v>798</v>
       </c>
@@ -33642,16 +33650,16 @@
         <v>931</v>
       </c>
       <c r="F413" s="25"/>
-      <c r="G413" s="28" t="s">
-        <v>1008</v>
-      </c>
-      <c r="H413" s="50" t="s">
-        <v>1009</v>
+      <c r="G413" s="42" t="s">
+        <v>994</v>
+      </c>
+      <c r="H413" s="43" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="414" spans="1:8" ht="50" customHeight="1">
-      <c r="A414" s="55"/>
-      <c r="B414" s="55"/>
+      <c r="A414" s="58"/>
+      <c r="B414" s="58"/>
       <c r="C414" s="27" t="s">
         <v>800</v>
       </c>
@@ -33670,8 +33678,8 @@
       </c>
     </row>
     <row r="415" spans="1:8" ht="50" customHeight="1">
-      <c r="A415" s="55"/>
-      <c r="B415" s="55"/>
+      <c r="A415" s="58"/>
+      <c r="B415" s="58"/>
       <c r="C415" s="27" t="s">
         <v>802</v>
       </c>
@@ -33690,8 +33698,8 @@
       </c>
     </row>
     <row r="416" spans="1:8" ht="50" customHeight="1">
-      <c r="A416" s="55"/>
-      <c r="B416" s="55"/>
+      <c r="A416" s="58"/>
+      <c r="B416" s="58"/>
       <c r="C416" s="27" t="s">
         <v>804</v>
       </c>
@@ -33710,8 +33718,8 @@
       </c>
     </row>
     <row r="417" spans="1:8" ht="50" customHeight="1">
-      <c r="A417" s="55"/>
-      <c r="B417" s="56"/>
+      <c r="A417" s="58"/>
+      <c r="B417" s="59"/>
       <c r="C417" s="27" t="s">
         <v>806</v>
       </c>
@@ -33730,8 +33738,8 @@
       </c>
     </row>
     <row r="418" spans="1:8" ht="50" customHeight="1">
-      <c r="A418" s="55"/>
-      <c r="B418" s="54" t="s">
+      <c r="A418" s="58"/>
+      <c r="B418" s="57" t="s">
         <v>865</v>
       </c>
       <c r="C418" s="26" t="s">
@@ -33751,8 +33759,8 @@
       </c>
     </row>
     <row r="419" spans="1:8" ht="50" customHeight="1">
-      <c r="A419" s="55"/>
-      <c r="B419" s="56"/>
+      <c r="A419" s="58"/>
+      <c r="B419" s="59"/>
       <c r="C419" s="27" t="s">
         <v>810</v>
       </c>
@@ -33770,8 +33778,8 @@
       </c>
     </row>
     <row r="420" spans="1:8" ht="50" customHeight="1">
-      <c r="A420" s="55"/>
-      <c r="B420" s="54" t="s">
+      <c r="A420" s="58"/>
+      <c r="B420" s="57" t="s">
         <v>866</v>
       </c>
       <c r="C420" s="26" t="s">
@@ -33791,8 +33799,8 @@
       </c>
     </row>
     <row r="421" spans="1:8" ht="50" customHeight="1">
-      <c r="A421" s="55"/>
-      <c r="B421" s="55"/>
+      <c r="A421" s="58"/>
+      <c r="B421" s="58"/>
       <c r="C421" s="26" t="s">
         <v>814</v>
       </c>
@@ -33810,8 +33818,8 @@
       </c>
     </row>
     <row r="422" spans="1:8" ht="50" customHeight="1">
-      <c r="A422" s="55"/>
-      <c r="B422" s="55"/>
+      <c r="A422" s="58"/>
+      <c r="B422" s="58"/>
       <c r="C422" s="26" t="s">
         <v>816</v>
       </c>
@@ -33829,8 +33837,8 @@
       </c>
     </row>
     <row r="423" spans="1:8" ht="50" customHeight="1">
-      <c r="A423" s="55"/>
-      <c r="B423" s="55"/>
+      <c r="A423" s="58"/>
+      <c r="B423" s="58"/>
       <c r="C423" s="26" t="s">
         <v>818</v>
       </c>
@@ -33848,8 +33856,8 @@
       </c>
     </row>
     <row r="424" spans="1:8" ht="50" customHeight="1">
-      <c r="A424" s="56"/>
-      <c r="B424" s="56"/>
+      <c r="A424" s="59"/>
+      <c r="B424" s="59"/>
       <c r="C424" s="26" t="s">
         <v>820</v>
       </c>
@@ -33869,31 +33877,15 @@
   </sheetData>
   <autoFilter ref="A2:H424" xr:uid="{54C32CA2-D16D-4A03-AF28-86A02BDF4FCA}"/>
   <mergeCells count="50">
-    <mergeCell ref="B48:B57"/>
-    <mergeCell ref="A34:A57"/>
-    <mergeCell ref="B34:B42"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A16:A33"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="A58:A70"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A71:A112"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B96"/>
-    <mergeCell ref="B97:B106"/>
-    <mergeCell ref="B107:B112"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A124:A147"/>
-    <mergeCell ref="B124:B138"/>
-    <mergeCell ref="B139:B147"/>
-    <mergeCell ref="B116:B123"/>
+    <mergeCell ref="B315:B317"/>
+    <mergeCell ref="B318:B327"/>
+    <mergeCell ref="B329:B333"/>
+    <mergeCell ref="B230:B231"/>
+    <mergeCell ref="B232:B233"/>
+    <mergeCell ref="B234:B268"/>
+    <mergeCell ref="B275:B307"/>
+    <mergeCell ref="B310:B314"/>
+    <mergeCell ref="B270:B274"/>
     <mergeCell ref="A148:A227"/>
     <mergeCell ref="A228:A333"/>
     <mergeCell ref="A334:A406"/>
@@ -33910,15 +33902,31 @@
     <mergeCell ref="B181:B186"/>
     <mergeCell ref="B187:B223"/>
     <mergeCell ref="B224:B227"/>
-    <mergeCell ref="B315:B317"/>
-    <mergeCell ref="B318:B327"/>
-    <mergeCell ref="B329:B333"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="B232:B233"/>
-    <mergeCell ref="B234:B268"/>
-    <mergeCell ref="B275:B307"/>
-    <mergeCell ref="B310:B314"/>
-    <mergeCell ref="B270:B274"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A124:A147"/>
+    <mergeCell ref="B124:B138"/>
+    <mergeCell ref="B139:B147"/>
+    <mergeCell ref="B116:B123"/>
+    <mergeCell ref="A58:A70"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A71:A112"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B74:B96"/>
+    <mergeCell ref="B97:B106"/>
+    <mergeCell ref="B107:B112"/>
+    <mergeCell ref="B48:B57"/>
+    <mergeCell ref="A34:A57"/>
+    <mergeCell ref="B34:B42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="A16:A33"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <conditionalFormatting sqref="E329:F329 E307:F308 E323:F327 E126:F126">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -33932,18 +33940,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34150,26 +34158,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E6096D8-1CD1-477D-852D-41029505002A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1765E8E-7B87-4E57-AE04-80D6CA061ADD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1750c493-bee6-4013-b7a9-faed7d1eacd9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fddf207-9565-4c1d-88a2-78ac3eb02019"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1765E8E-7B87-4E57-AE04-80D6CA061ADD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E6096D8-1CD1-477D-852D-41029505002A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1750c493-bee6-4013-b7a9-faed7d1eacd9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0fddf207-9565-4c1d-88a2-78ac3eb02019"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>